<commit_message>
feat: added incremental way of training the model
</commit_message>
<xml_diff>
--- a/src/data/raw/BSOFT.NS_data.xlsx
+++ b/src/data/raw/BSOFT.NS_data.xlsx
@@ -461,16 +461,16 @@
         <v>44929</v>
       </c>
       <c r="B2" t="n">
-        <v>292.9236450195312</v>
+        <v>292.9236755371094</v>
       </c>
       <c r="C2" t="n">
-        <v>293.6569318329125</v>
+        <v>293.6569624268864</v>
       </c>
       <c r="D2" t="n">
-        <v>285.7863021334437</v>
+        <v>285.7863319074341</v>
       </c>
       <c r="E2" t="n">
-        <v>287.9372887210354</v>
+        <v>287.9373187191214</v>
       </c>
       <c r="F2" t="n">
         <v>2515189</v>
@@ -481,16 +481,16 @@
         <v>44930</v>
       </c>
       <c r="B3" t="n">
-        <v>288.1817016601562</v>
+        <v>288.1817626953125</v>
       </c>
       <c r="C3" t="n">
-        <v>293.2169315316686</v>
+        <v>293.2169936332564</v>
       </c>
       <c r="D3" t="n">
-        <v>286.1284927291712</v>
+        <v>286.1285533294701</v>
       </c>
       <c r="E3" t="n">
-        <v>293.2169315316686</v>
+        <v>293.2169936332564</v>
       </c>
       <c r="F3" t="n">
         <v>1599439</v>
@@ -521,16 +521,16 @@
         <v>44932</v>
       </c>
       <c r="B5" t="n">
-        <v>277.3291015625</v>
+        <v>277.3290710449219</v>
       </c>
       <c r="C5" t="n">
-        <v>285.0041771373037</v>
+        <v>285.0041457751524</v>
       </c>
       <c r="D5" t="n">
-        <v>276.4491632438169</v>
+        <v>276.4491328230681</v>
       </c>
       <c r="E5" t="n">
-        <v>284.4175416456748</v>
+        <v>284.4175103480775</v>
       </c>
       <c r="F5" t="n">
         <v>2295178</v>
@@ -541,16 +541,16 @@
         <v>44935</v>
       </c>
       <c r="B6" t="n">
-        <v>287.1062622070312</v>
+        <v>287.1062316894531</v>
       </c>
       <c r="C6" t="n">
-        <v>288.3773107535992</v>
+        <v>288.3772801009167</v>
       </c>
       <c r="D6" t="n">
-        <v>280.9955379567645</v>
+        <v>280.9955080887176</v>
       </c>
       <c r="E6" t="n">
-        <v>280.9955379567645</v>
+        <v>280.9955080887176</v>
       </c>
       <c r="F6" t="n">
         <v>3174952</v>
@@ -581,16 +581,16 @@
         <v>44937</v>
       </c>
       <c r="B8" t="n">
-        <v>287.7417602539062</v>
+        <v>287.7417297363281</v>
       </c>
       <c r="C8" t="n">
-        <v>291.3104469458368</v>
+        <v>291.3104160497676</v>
       </c>
       <c r="D8" t="n">
-        <v>284.0264519907562</v>
+        <v>284.0264218672196</v>
       </c>
       <c r="E8" t="n">
-        <v>285.3463743444478</v>
+        <v>285.3463440809217</v>
       </c>
       <c r="F8" t="n">
         <v>1536020</v>
@@ -621,16 +621,16 @@
         <v>44939</v>
       </c>
       <c r="B10" t="n">
-        <v>287.1551818847656</v>
+        <v>287.1551513671875</v>
       </c>
       <c r="C10" t="n">
-        <v>288.4262006645496</v>
+        <v>288.4261700118932</v>
       </c>
       <c r="D10" t="n">
-        <v>280.8977760342286</v>
+        <v>280.8977461816598</v>
       </c>
       <c r="E10" t="n">
-        <v>286.2752136737372</v>
+        <v>286.2751832496782</v>
       </c>
       <c r="F10" t="n">
         <v>2186938</v>
@@ -661,16 +661,16 @@
         <v>44943</v>
       </c>
       <c r="B12" t="n">
-        <v>289.6483154296875</v>
+        <v>289.6483459472656</v>
       </c>
       <c r="C12" t="n">
-        <v>292.8258918858781</v>
+        <v>292.8259227382483</v>
       </c>
       <c r="D12" t="n">
-        <v>288.426170638845</v>
+        <v>288.4262010276569</v>
       </c>
       <c r="E12" t="n">
-        <v>290.3816023041931</v>
+        <v>290.3816328990309</v>
       </c>
       <c r="F12" t="n">
         <v>1047676</v>
@@ -681,16 +681,16 @@
         <v>44944</v>
       </c>
       <c r="B13" t="n">
-        <v>288.1817016601562</v>
+        <v>288.1817626953125</v>
       </c>
       <c r="C13" t="n">
-        <v>292.2392158347724</v>
+        <v>292.2392777292859</v>
       </c>
       <c r="D13" t="n">
-        <v>287.5461924246767</v>
+        <v>287.546253325236</v>
       </c>
       <c r="E13" t="n">
-        <v>290.3815619781727</v>
+        <v>290.3816234792462</v>
       </c>
       <c r="F13" t="n">
         <v>1004351</v>
@@ -701,16 +701,16 @@
         <v>44945</v>
       </c>
       <c r="B14" t="n">
-        <v>288.2305908203125</v>
+        <v>288.2306213378906</v>
       </c>
       <c r="C14" t="n">
-        <v>289.061655174322</v>
+        <v>289.0616857798925</v>
       </c>
       <c r="D14" t="n">
-        <v>283.9286474929604</v>
+        <v>283.9286775550528</v>
       </c>
       <c r="E14" t="n">
-        <v>286.5195882598586</v>
+        <v>286.5196185962774</v>
       </c>
       <c r="F14" t="n">
         <v>755390</v>
@@ -741,16 +741,16 @@
         <v>44949</v>
       </c>
       <c r="B16" t="n">
-        <v>295.95458984375</v>
+        <v>295.9546203613281</v>
       </c>
       <c r="C16" t="n">
-        <v>297.4211635697596</v>
+        <v>297.4211942385646</v>
       </c>
       <c r="D16" t="n">
-        <v>285.0041607545372</v>
+        <v>285.0041901429537</v>
       </c>
       <c r="E16" t="n">
-        <v>287.5951017029838</v>
+        <v>287.5951313585671</v>
       </c>
       <c r="F16" t="n">
         <v>2610113</v>
@@ -781,16 +781,16 @@
         <v>44951</v>
       </c>
       <c r="B18" t="n">
-        <v>289.3550109863281</v>
+        <v>289.3550415039062</v>
       </c>
       <c r="C18" t="n">
-        <v>299.1810431143912</v>
+        <v>299.1810746682973</v>
       </c>
       <c r="D18" t="n">
-        <v>288.3283914652869</v>
+        <v>288.3284218745899</v>
       </c>
       <c r="E18" t="n">
-        <v>299.1810431143912</v>
+        <v>299.1810746682973</v>
       </c>
       <c r="F18" t="n">
         <v>1965674</v>
@@ -821,16 +821,16 @@
         <v>44956</v>
       </c>
       <c r="B20" t="n">
-        <v>288.2305908203125</v>
+        <v>288.2306213378906</v>
       </c>
       <c r="C20" t="n">
-        <v>292.3370089004085</v>
+        <v>292.3370398527703</v>
       </c>
       <c r="D20" t="n">
-        <v>280.6044199144389</v>
+        <v>280.6044496245655</v>
       </c>
       <c r="E20" t="n">
-        <v>284.564156762197</v>
+        <v>284.5641868915766</v>
       </c>
       <c r="F20" t="n">
         <v>1560058</v>
@@ -861,16 +861,16 @@
         <v>44958</v>
       </c>
       <c r="B22" t="n">
-        <v>289.4039001464844</v>
+        <v>289.4039306640625</v>
       </c>
       <c r="C22" t="n">
-        <v>298.9366299654986</v>
+        <v>298.936661488301</v>
       </c>
       <c r="D22" t="n">
-        <v>284.661972166445</v>
+        <v>284.6620021839878</v>
       </c>
       <c r="E22" t="n">
-        <v>296.9323243488167</v>
+        <v>296.9323556602656</v>
       </c>
       <c r="F22" t="n">
         <v>1939798</v>
@@ -921,16 +921,16 @@
         <v>44963</v>
       </c>
       <c r="B25" t="n">
-        <v>277.4757690429688</v>
+        <v>277.4757385253906</v>
       </c>
       <c r="C25" t="n">
-        <v>278.4534849731237</v>
+        <v>278.4534543480136</v>
       </c>
       <c r="D25" t="n">
-        <v>260.4146439642781</v>
+        <v>260.4146153231312</v>
       </c>
       <c r="E25" t="n">
-        <v>262.8589337896655</v>
+        <v>262.8589048796886</v>
       </c>
       <c r="F25" t="n">
         <v>4371731</v>
@@ -981,16 +981,16 @@
         <v>44966</v>
       </c>
       <c r="B28" t="n">
-        <v>281.8754577636719</v>
+        <v>281.87548828125</v>
       </c>
       <c r="C28" t="n">
-        <v>282.7554258679179</v>
+        <v>282.7554564807669</v>
       </c>
       <c r="D28" t="n">
-        <v>277.4757365925166</v>
+        <v>277.4757666337538</v>
       </c>
       <c r="E28" t="n">
-        <v>281.0444231902464</v>
+        <v>281.0444536178517</v>
       </c>
       <c r="F28" t="n">
         <v>1510346</v>
@@ -1001,16 +1001,16 @@
         <v>44967</v>
       </c>
       <c r="B29" t="n">
-        <v>285.9330139160156</v>
+        <v>285.9329833984375</v>
       </c>
       <c r="C29" t="n">
-        <v>286.6663008077433</v>
+        <v>286.6662702119016</v>
       </c>
       <c r="D29" t="n">
-        <v>277.1824450730575</v>
+        <v>277.182415489426</v>
       </c>
       <c r="E29" t="n">
-        <v>279.8222898182851</v>
+        <v>279.8222599529034</v>
       </c>
       <c r="F29" t="n">
         <v>1732448</v>
@@ -1021,16 +1021,16 @@
         <v>44970</v>
       </c>
       <c r="B30" t="n">
-        <v>281.1422119140625</v>
+        <v>281.1421508789062</v>
       </c>
       <c r="C30" t="n">
-        <v>284.8086467582079</v>
+        <v>284.8085849270793</v>
       </c>
       <c r="D30" t="n">
-        <v>276.7913938015238</v>
+        <v>276.7913337109175</v>
       </c>
       <c r="E30" t="n">
-        <v>284.0264859264662</v>
+        <v>284.0264242651424</v>
       </c>
       <c r="F30" t="n">
         <v>3345334</v>
@@ -1041,16 +1041,16 @@
         <v>44971</v>
       </c>
       <c r="B31" t="n">
-        <v>281.3865661621094</v>
+        <v>281.3866271972656</v>
       </c>
       <c r="C31" t="n">
-        <v>288.3283535906601</v>
+        <v>288.3284161315495</v>
       </c>
       <c r="D31" t="n">
-        <v>280.6044055381242</v>
+        <v>280.6044664036231</v>
       </c>
       <c r="E31" t="n">
-        <v>282.5598369356024</v>
+        <v>282.5598982252511</v>
       </c>
       <c r="F31" t="n">
         <v>1826849</v>
@@ -1061,16 +1061,16 @@
         <v>44972</v>
       </c>
       <c r="B32" t="n">
-        <v>286.5195922851562</v>
+        <v>286.5196228027344</v>
       </c>
       <c r="C32" t="n">
-        <v>289.061659235333</v>
+        <v>289.0616900236701</v>
       </c>
       <c r="D32" t="n">
-        <v>278.160134450218</v>
+        <v>278.1601640774194</v>
       </c>
       <c r="E32" t="n">
-        <v>280.1155659753514</v>
+        <v>280.1155958108283</v>
       </c>
       <c r="F32" t="n">
         <v>1518654</v>
@@ -1181,16 +1181,16 @@
         <v>44980</v>
       </c>
       <c r="B38" t="n">
-        <v>276.7424621582031</v>
+        <v>276.742431640625</v>
       </c>
       <c r="C38" t="n">
-        <v>278.8445751266132</v>
+        <v>278.844544377226</v>
       </c>
       <c r="D38" t="n">
-        <v>273.222708933234</v>
+        <v>273.2226788037942</v>
       </c>
       <c r="E38" t="n">
-        <v>277.5246527484897</v>
+        <v>277.5246221446561</v>
       </c>
       <c r="F38" t="n">
         <v>1796972</v>
@@ -1201,16 +1201,16 @@
         <v>44981</v>
       </c>
       <c r="B39" t="n">
-        <v>276.6446838378906</v>
+        <v>276.6447143554688</v>
       </c>
       <c r="C39" t="n">
-        <v>281.0932785724655</v>
+        <v>281.0933095807827</v>
       </c>
       <c r="D39" t="n">
-        <v>275.8624933341354</v>
+        <v>275.8625237654276</v>
       </c>
       <c r="E39" t="n">
-        <v>278.1601313177963</v>
+        <v>278.1601620025484</v>
       </c>
       <c r="F39" t="n">
         <v>629355</v>
@@ -1261,16 +1261,16 @@
         <v>44986</v>
       </c>
       <c r="B42" t="n">
-        <v>270.8272705078125</v>
+        <v>270.8273010253906</v>
       </c>
       <c r="C42" t="n">
-        <v>272.8315759177189</v>
+        <v>272.8316066611478</v>
       </c>
       <c r="D42" t="n">
-        <v>268.2363296635987</v>
+        <v>268.2363598892223</v>
       </c>
       <c r="E42" t="n">
-        <v>269.849554729806</v>
+        <v>269.8495851372123</v>
       </c>
       <c r="F42" t="n">
         <v>1276137</v>
@@ -1321,16 +1321,16 @@
         <v>44991</v>
       </c>
       <c r="B45" t="n">
-        <v>281.8265686035156</v>
+        <v>281.8265991210938</v>
       </c>
       <c r="C45" t="n">
-        <v>287.4484342391452</v>
+        <v>287.4484653654868</v>
       </c>
       <c r="D45" t="n">
-        <v>275.7647189396561</v>
+        <v>275.764748800827</v>
       </c>
       <c r="E45" t="n">
-        <v>275.7647189396561</v>
+        <v>275.764748800827</v>
       </c>
       <c r="F45" t="n">
         <v>3394370</v>
@@ -1341,16 +1341,16 @@
         <v>44993</v>
       </c>
       <c r="B46" t="n">
-        <v>279.7244873046875</v>
+        <v>279.7245178222656</v>
       </c>
       <c r="C46" t="n">
-        <v>283.195366347475</v>
+        <v>283.1953972437216</v>
       </c>
       <c r="D46" t="n">
-        <v>275.1292112582344</v>
+        <v>275.1292412744738</v>
       </c>
       <c r="E46" t="n">
-        <v>283.195366347475</v>
+        <v>283.1953972437216</v>
       </c>
       <c r="F46" t="n">
         <v>1358145</v>
@@ -1361,16 +1361,16 @@
         <v>44994</v>
       </c>
       <c r="B47" t="n">
-        <v>275.0314331054688</v>
+        <v>275.0314636230469</v>
       </c>
       <c r="C47" t="n">
-        <v>282.706507837877</v>
+        <v>282.706539207084</v>
       </c>
       <c r="D47" t="n">
-        <v>274.3959238249228</v>
+        <v>274.3959542719846</v>
       </c>
       <c r="E47" t="n">
-        <v>280.7999799962391</v>
+        <v>280.8000111538971</v>
       </c>
       <c r="F47" t="n">
         <v>943696</v>
@@ -1481,16 +1481,16 @@
         <v>45002</v>
       </c>
       <c r="B53" t="n">
-        <v>270.3873291015625</v>
+        <v>270.3872680664062</v>
       </c>
       <c r="C53" t="n">
-        <v>271.6094740167522</v>
+        <v>271.6094127057183</v>
       </c>
       <c r="D53" t="n">
-        <v>267.6986102881451</v>
+        <v>267.6985498599196</v>
       </c>
       <c r="E53" t="n">
-        <v>268.2852458149407</v>
+        <v>268.2851852542925</v>
       </c>
       <c r="F53" t="n">
         <v>907042</v>
@@ -1501,16 +1501,16 @@
         <v>45005</v>
       </c>
       <c r="B54" t="n">
-        <v>266.9164123535156</v>
+        <v>266.9164428710938</v>
       </c>
       <c r="C54" t="n">
-        <v>269.6540046477752</v>
+        <v>269.6540354783527</v>
       </c>
       <c r="D54" t="n">
-        <v>259.3391149332235</v>
+        <v>259.3391445844601</v>
       </c>
       <c r="E54" t="n">
-        <v>268.8718439458491</v>
+        <v>268.8718746869992</v>
       </c>
       <c r="F54" t="n">
         <v>1007637</v>
@@ -1561,16 +1561,16 @@
         <v>45008</v>
       </c>
       <c r="B57" t="n">
-        <v>262.02783203125</v>
+        <v>262.0278625488281</v>
       </c>
       <c r="C57" t="n">
-        <v>266.525330638096</v>
+        <v>266.525361679484</v>
       </c>
       <c r="D57" t="n">
-        <v>261.3434190424298</v>
+        <v>261.3434494802965</v>
       </c>
       <c r="E57" t="n">
-        <v>263.3477543168215</v>
+        <v>263.3477849881269</v>
       </c>
       <c r="F57" t="n">
         <v>1320289</v>
@@ -1581,16 +1581,16 @@
         <v>45009</v>
       </c>
       <c r="B58" t="n">
-        <v>258.8013610839844</v>
+        <v>258.8013916015625</v>
       </c>
       <c r="C58" t="n">
-        <v>268.3340892827095</v>
+        <v>268.3341209243766</v>
       </c>
       <c r="D58" t="n">
-        <v>257.1881062880337</v>
+        <v>257.1881366153786</v>
       </c>
       <c r="E58" t="n">
-        <v>263.3477331804886</v>
+        <v>263.34776423417</v>
       </c>
       <c r="F58" t="n">
         <v>2453889</v>
@@ -1601,16 +1601,16 @@
         <v>45012</v>
       </c>
       <c r="B59" t="n">
-        <v>255.0372009277344</v>
+        <v>255.0371704101562</v>
       </c>
       <c r="C59" t="n">
-        <v>260.5612898481936</v>
+        <v>260.5612586696068</v>
       </c>
       <c r="D59" t="n">
-        <v>254.2061364372621</v>
+        <v>254.2061060191286</v>
       </c>
       <c r="E59" t="n">
-        <v>260.1702094519483</v>
+        <v>260.1701783201579</v>
       </c>
       <c r="F59" t="n">
         <v>1101294</v>
@@ -1641,16 +1641,16 @@
         <v>45014</v>
       </c>
       <c r="B61" t="n">
-        <v>249.8063812255859</v>
+        <v>249.806396484375</v>
       </c>
       <c r="C61" t="n">
-        <v>250.9796520939421</v>
+        <v>250.9796674243975</v>
       </c>
       <c r="D61" t="n">
-        <v>244.9178023366312</v>
+        <v>244.9178172968138</v>
       </c>
       <c r="E61" t="n">
-        <v>247.3620917811086</v>
+        <v>247.3621068905944</v>
       </c>
       <c r="F61" t="n">
         <v>1292904</v>
@@ -1661,16 +1661,16 @@
         <v>45016</v>
       </c>
       <c r="B62" t="n">
-        <v>255.3304595947266</v>
+        <v>255.3305053710938</v>
       </c>
       <c r="C62" t="n">
-        <v>256.6992556635515</v>
+        <v>256.6993016853203</v>
       </c>
       <c r="D62" t="n">
-        <v>251.6640255688473</v>
+        <v>251.6640706878859</v>
       </c>
       <c r="E62" t="n">
-        <v>251.8106769623792</v>
+        <v>251.8107221077098</v>
       </c>
       <c r="F62" t="n">
         <v>1436959</v>
@@ -1681,16 +1681,16 @@
         <v>45019</v>
       </c>
       <c r="B63" t="n">
-        <v>260.7568359375</v>
+        <v>260.7568054199219</v>
       </c>
       <c r="C63" t="n">
-        <v>261.9789807819061</v>
+        <v>261.9789501212948</v>
       </c>
       <c r="D63" t="n">
-        <v>254.792763129294</v>
+        <v>254.7927333097189</v>
       </c>
       <c r="E63" t="n">
-        <v>258.605849076337</v>
+        <v>258.6058188104988</v>
       </c>
       <c r="F63" t="n">
         <v>1008929</v>
@@ -1721,16 +1721,16 @@
         <v>45022</v>
       </c>
       <c r="B65" t="n">
-        <v>260.0723876953125</v>
+        <v>260.0724182128906</v>
       </c>
       <c r="C65" t="n">
-        <v>262.4188995115263</v>
+        <v>262.4189303044503</v>
       </c>
       <c r="D65" t="n">
-        <v>258.7035916223141</v>
+        <v>258.7036219792741</v>
       </c>
       <c r="E65" t="n">
-        <v>260.0723876953125</v>
+        <v>260.0724182128906</v>
       </c>
       <c r="F65" t="n">
         <v>748621</v>
@@ -1761,16 +1761,16 @@
         <v>45027</v>
       </c>
       <c r="B67" t="n">
-        <v>259.8768920898438</v>
+        <v>259.8768310546875</v>
       </c>
       <c r="C67" t="n">
-        <v>263.2500241109545</v>
+        <v>263.2499622835784</v>
       </c>
       <c r="D67" t="n">
-        <v>259.0947312512644</v>
+        <v>259.0946703998079</v>
       </c>
       <c r="E67" t="n">
-        <v>261.5390211687292</v>
+        <v>261.5389597432023</v>
       </c>
       <c r="F67" t="n">
         <v>852555</v>
@@ -1781,16 +1781,16 @@
         <v>45028</v>
       </c>
       <c r="B68" t="n">
-        <v>263.7877502441406</v>
+        <v>263.7877197265625</v>
       </c>
       <c r="C68" t="n">
-        <v>264.7165923276679</v>
+        <v>264.7165617026321</v>
       </c>
       <c r="D68" t="n">
-        <v>259.5835836121729</v>
+        <v>259.5835535809744</v>
       </c>
       <c r="E68" t="n">
-        <v>260.267996709248</v>
+        <v>260.2679665988698</v>
       </c>
       <c r="F68" t="n">
         <v>717121</v>
@@ -1801,16 +1801,16 @@
         <v>45029</v>
       </c>
       <c r="B69" t="n">
-        <v>257.237060546875</v>
+        <v>257.2370300292969</v>
       </c>
       <c r="C69" t="n">
-        <v>263.1033559762791</v>
+        <v>263.1033247627471</v>
       </c>
       <c r="D69" t="n">
-        <v>256.3082185022108</v>
+        <v>256.3081880948267</v>
       </c>
       <c r="E69" t="n">
-        <v>261.343449444945</v>
+        <v>261.3434184402013</v>
       </c>
       <c r="F69" t="n">
         <v>1119774</v>
@@ -1821,16 +1821,16 @@
         <v>45033</v>
       </c>
       <c r="B70" t="n">
-        <v>252.7883911132812</v>
+        <v>252.7884063720703</v>
       </c>
       <c r="C70" t="n">
-        <v>254.0105357808905</v>
+        <v>254.0105511134505</v>
       </c>
       <c r="D70" t="n">
-        <v>246.2865874491035</v>
+        <v>246.2866023154313</v>
       </c>
       <c r="E70" t="n">
-        <v>251.761801527496</v>
+        <v>251.7618167243182</v>
       </c>
       <c r="F70" t="n">
         <v>1947730</v>
@@ -1861,16 +1861,16 @@
         <v>45035</v>
       </c>
       <c r="B72" t="n">
-        <v>252.3484497070312</v>
+        <v>252.3484649658203</v>
       </c>
       <c r="C72" t="n">
-        <v>258.7524761544104</v>
+        <v>258.7524918004327</v>
       </c>
       <c r="D72" t="n">
-        <v>251.4685114693214</v>
+        <v>251.4685266749031</v>
       </c>
       <c r="E72" t="n">
-        <v>258.4102696626572</v>
+        <v>258.4102852879872</v>
       </c>
       <c r="F72" t="n">
         <v>1542730</v>
@@ -1881,16 +1881,16 @@
         <v>45036</v>
       </c>
       <c r="B73" t="n">
-        <v>253.130615234375</v>
+        <v>253.1305999755859</v>
       </c>
       <c r="C73" t="n">
-        <v>254.4505375349128</v>
+        <v>254.4505221965584</v>
       </c>
       <c r="D73" t="n">
-        <v>250.9796583719415</v>
+        <v>250.9796432428128</v>
       </c>
       <c r="E73" t="n">
-        <v>252.4951059304178</v>
+        <v>252.4950907099374</v>
       </c>
       <c r="F73" t="n">
         <v>903815</v>
@@ -1901,16 +1901,16 @@
         <v>45037</v>
       </c>
       <c r="B74" t="n">
-        <v>251.27294921875</v>
+        <v>251.2729644775391</v>
       </c>
       <c r="C74" t="n">
-        <v>254.6460805109735</v>
+        <v>254.6460959745991</v>
       </c>
       <c r="D74" t="n">
-        <v>250.0996932956437</v>
+        <v>250.0997084831857</v>
       </c>
       <c r="E74" t="n">
-        <v>253.6194610649626</v>
+        <v>253.6194764662458</v>
       </c>
       <c r="F74" t="n">
         <v>911187</v>
@@ -1941,16 +1941,16 @@
         <v>45041</v>
       </c>
       <c r="B76" t="n">
-        <v>259.339111328125</v>
+        <v>259.3391418457031</v>
       </c>
       <c r="C76" t="n">
-        <v>263.7388323497143</v>
+        <v>263.738863385027</v>
       </c>
       <c r="D76" t="n">
-        <v>255.4282481978234</v>
+        <v>255.428278255193</v>
       </c>
       <c r="E76" t="n">
-        <v>259.2902374740033</v>
+        <v>259.2902679858303</v>
       </c>
       <c r="F76" t="n">
         <v>1594968</v>
@@ -1981,16 +1981,16 @@
         <v>45043</v>
       </c>
       <c r="B78" t="n">
-        <v>265.1565246582031</v>
+        <v>265.1565551757812</v>
       </c>
       <c r="C78" t="n">
-        <v>269.1651353831937</v>
+        <v>269.1651663621336</v>
       </c>
       <c r="D78" t="n">
-        <v>258.8502461042265</v>
+        <v>258.8502758959981</v>
       </c>
       <c r="E78" t="n">
-        <v>262.0278223075834</v>
+        <v>262.0278524650707</v>
       </c>
       <c r="F78" t="n">
         <v>2306301</v>
@@ -2001,16 +2001,16 @@
         <v>45044</v>
       </c>
       <c r="B79" t="n">
-        <v>266.8675231933594</v>
+        <v>266.8675537109375</v>
       </c>
       <c r="C79" t="n">
-        <v>271.7561018938238</v>
+        <v>271.7561329704343</v>
       </c>
       <c r="D79" t="n">
-        <v>265.3031720417075</v>
+        <v>265.3032023803946</v>
       </c>
       <c r="E79" t="n">
-        <v>266.9163970453574</v>
+        <v>266.9164275685245</v>
       </c>
       <c r="F79" t="n">
         <v>2199682</v>
@@ -2021,16 +2021,16 @@
         <v>45048</v>
       </c>
       <c r="B80" t="n">
-        <v>272.0982971191406</v>
+        <v>272.0983276367188</v>
       </c>
       <c r="C80" t="n">
-        <v>274.1515062810881</v>
+        <v>274.1515370289469</v>
       </c>
       <c r="D80" t="n">
-        <v>266.9652891330311</v>
+        <v>266.9653190749093</v>
       </c>
       <c r="E80" t="n">
-        <v>268.3829889880116</v>
+        <v>268.383019088894</v>
       </c>
       <c r="F80" t="n">
         <v>2686833</v>
@@ -2041,16 +2041,16 @@
         <v>45049</v>
       </c>
       <c r="B81" t="n">
-        <v>269.4095764160156</v>
+        <v>269.4096069335938</v>
       </c>
       <c r="C81" t="n">
-        <v>273.2226919012325</v>
+        <v>273.2227228507442</v>
       </c>
       <c r="D81" t="n">
-        <v>267.454144818476</v>
+        <v>267.454175114551</v>
       </c>
       <c r="E81" t="n">
-        <v>272.2449761024627</v>
+        <v>272.2450069412229</v>
       </c>
       <c r="F81" t="n">
         <v>1040500</v>
@@ -2061,16 +2061,16 @@
         <v>45050</v>
       </c>
       <c r="B82" t="n">
-        <v>280.6044311523438</v>
+        <v>280.6044616699219</v>
       </c>
       <c r="C82" t="n">
-        <v>281.7777020329356</v>
+        <v>281.7777326781147</v>
       </c>
       <c r="D82" t="n">
-        <v>268.9207155508888</v>
+        <v>268.920744797786</v>
       </c>
       <c r="E82" t="n">
-        <v>269.4095734448824</v>
+        <v>269.4096027449461</v>
       </c>
       <c r="F82" t="n">
         <v>3084961</v>
@@ -2081,16 +2081,16 @@
         <v>45051</v>
       </c>
       <c r="B83" t="n">
-        <v>275.3736267089844</v>
+        <v>275.3736572265625</v>
       </c>
       <c r="C83" t="n">
-        <v>282.2176367524263</v>
+        <v>282.2176680284743</v>
       </c>
       <c r="D83" t="n">
-        <v>274.2981334489403</v>
+        <v>274.2981638473296</v>
       </c>
       <c r="E83" t="n">
-        <v>280.6044117811181</v>
+        <v>280.6044428783846</v>
       </c>
       <c r="F83" t="n">
         <v>1642424</v>
@@ -2101,16 +2101,16 @@
         <v>45054</v>
       </c>
       <c r="B84" t="n">
-        <v>281.3377075195312</v>
+        <v>281.3377380371094</v>
       </c>
       <c r="C84" t="n">
-        <v>282.4620746663545</v>
+        <v>282.4621053058962</v>
       </c>
       <c r="D84" t="n">
-        <v>274.3470458631783</v>
+        <v>274.3470756224576</v>
       </c>
       <c r="E84" t="n">
-        <v>277.9157023889722</v>
+        <v>277.9157325353548</v>
       </c>
       <c r="F84" t="n">
         <v>2382236</v>
@@ -2121,16 +2121,16 @@
         <v>45055</v>
       </c>
       <c r="B85" t="n">
-        <v>301.3808898925781</v>
+        <v>301.3809204101562</v>
       </c>
       <c r="C85" t="n">
-        <v>306.6116752953624</v>
+        <v>306.6117063426055</v>
       </c>
       <c r="D85" t="n">
-        <v>285.9329924673169</v>
+        <v>285.9330214206537</v>
       </c>
       <c r="E85" t="n">
-        <v>292.3370189063451</v>
+        <v>292.3370485081483</v>
       </c>
       <c r="F85" t="n">
         <v>20222326</v>
@@ -2141,16 +2141,16 @@
         <v>45056</v>
       </c>
       <c r="B86" t="n">
-        <v>300.1587524414062</v>
+        <v>300.1587829589844</v>
       </c>
       <c r="C86" t="n">
-        <v>305.0473314713966</v>
+        <v>305.0473624860036</v>
       </c>
       <c r="D86" t="n">
-        <v>294.9768706046239</v>
+        <v>294.9769005953526</v>
       </c>
       <c r="E86" t="n">
-        <v>302.1141840534024</v>
+        <v>302.1142147697921</v>
       </c>
       <c r="F86" t="n">
         <v>4394968</v>
@@ -2221,16 +2221,16 @@
         <v>45062</v>
       </c>
       <c r="B90" t="n">
-        <v>321.0330200195312</v>
+        <v>321.032958984375</v>
       </c>
       <c r="C90" t="n">
-        <v>327.045966804943</v>
+        <v>327.0459046265986</v>
       </c>
       <c r="D90" t="n">
-        <v>300.989844176478</v>
+        <v>300.9897869519527</v>
       </c>
       <c r="E90" t="n">
-        <v>302.6030694353658</v>
+        <v>302.6030119041324</v>
       </c>
       <c r="F90" t="n">
         <v>16881729</v>
@@ -2241,16 +2241,16 @@
         <v>45063</v>
       </c>
       <c r="B91" t="n">
-        <v>313.8956298828125</v>
+        <v>313.8956604003906</v>
       </c>
       <c r="C91" t="n">
-        <v>320.6907662863875</v>
+        <v>320.6907974646027</v>
       </c>
       <c r="D91" t="n">
-        <v>309.3981612988095</v>
+        <v>309.3981913791345</v>
       </c>
       <c r="E91" t="n">
-        <v>320.6907662863875</v>
+        <v>320.6907974646027</v>
       </c>
       <c r="F91" t="n">
         <v>5372474</v>
@@ -2261,16 +2261,16 @@
         <v>45064</v>
       </c>
       <c r="B92" t="n">
-        <v>311.8913269042969</v>
+        <v>311.891357421875</v>
       </c>
       <c r="C92" t="n">
-        <v>322.2551199099995</v>
+        <v>322.2551514416419</v>
       </c>
       <c r="D92" t="n">
-        <v>310.8158336026407</v>
+        <v>310.8158640149852</v>
       </c>
       <c r="E92" t="n">
-        <v>315.3133320584192</v>
+        <v>315.3133629108297</v>
       </c>
       <c r="F92" t="n">
         <v>2825454</v>
@@ -2281,16 +2281,16 @@
         <v>45065</v>
       </c>
       <c r="B93" t="n">
-        <v>327.1925659179688</v>
+        <v>327.1925964355469</v>
       </c>
       <c r="C93" t="n">
-        <v>329.8324103468967</v>
+        <v>329.8324411106957</v>
       </c>
       <c r="D93" t="n">
-        <v>312.9668138579548</v>
+        <v>312.9668430486828</v>
       </c>
       <c r="E93" t="n">
-        <v>313.846752055092</v>
+        <v>313.8467813278926</v>
       </c>
       <c r="F93" t="n">
         <v>10244689</v>
@@ -2301,16 +2301,16 @@
         <v>45068</v>
       </c>
       <c r="B94" t="n">
-        <v>332.5211791992188</v>
+        <v>332.5211486816406</v>
       </c>
       <c r="C94" t="n">
-        <v>333.4011175301813</v>
+        <v>333.4010869318457</v>
       </c>
       <c r="D94" t="n">
-        <v>324.7972296579592</v>
+        <v>324.797199849257</v>
       </c>
       <c r="E94" t="n">
-        <v>327.1926156790506</v>
+        <v>327.1925856505085</v>
       </c>
       <c r="F94" t="n">
         <v>3643637</v>
@@ -2341,16 +2341,16 @@
         <v>45070</v>
       </c>
       <c r="B96" t="n">
-        <v>323.4284057617188</v>
+        <v>323.4283752441406</v>
       </c>
       <c r="C96" t="n">
-        <v>329.2458272653352</v>
+        <v>329.2457961988455</v>
       </c>
       <c r="D96" t="n">
-        <v>317.7576655122018</v>
+        <v>317.7576355296949</v>
       </c>
       <c r="E96" t="n">
-        <v>326.9970926444112</v>
+        <v>326.9970617901042</v>
       </c>
       <c r="F96" t="n">
         <v>1588833</v>
@@ -2361,16 +2361,16 @@
         <v>45071</v>
       </c>
       <c r="B97" t="n">
-        <v>327.9258728027344</v>
+        <v>327.9259033203125</v>
       </c>
       <c r="C97" t="n">
-        <v>331.8367359961779</v>
+        <v>331.8367668777104</v>
       </c>
       <c r="D97" t="n">
-        <v>320.0552725609366</v>
+        <v>320.0553023460575</v>
       </c>
       <c r="E97" t="n">
-        <v>324.1127871566306</v>
+        <v>324.1128173193537</v>
       </c>
       <c r="F97" t="n">
         <v>2917161</v>
@@ -2381,16 +2381,16 @@
         <v>45072</v>
       </c>
       <c r="B98" t="n">
-        <v>331.9345092773438</v>
+        <v>331.9345397949219</v>
       </c>
       <c r="C98" t="n">
-        <v>336.3342303134205</v>
+        <v>336.3342612355026</v>
       </c>
       <c r="D98" t="n">
-        <v>327.7303433334332</v>
+        <v>327.7303734644863</v>
       </c>
       <c r="E98" t="n">
-        <v>330.2235066522028</v>
+        <v>330.2235370124738</v>
       </c>
       <c r="F98" t="n">
         <v>4851118</v>
@@ -2481,16 +2481,16 @@
         <v>45079</v>
       </c>
       <c r="B103" t="n">
-        <v>340.0495300292969</v>
+        <v>340.0495910644531</v>
       </c>
       <c r="C103" t="n">
-        <v>347.5290794773064</v>
+        <v>347.5291418549596</v>
       </c>
       <c r="D103" t="n">
-        <v>337.8007957120959</v>
+        <v>337.800856343629</v>
       </c>
       <c r="E103" t="n">
-        <v>338.240779739926</v>
+        <v>338.2408404504314</v>
       </c>
       <c r="F103" t="n">
         <v>4103271</v>
@@ -2581,16 +2581,16 @@
         <v>45086</v>
       </c>
       <c r="B108" t="n">
-        <v>321.1796264648438</v>
+        <v>321.1796569824219</v>
       </c>
       <c r="C108" t="n">
-        <v>329.7835131992148</v>
+        <v>329.7835445343098</v>
       </c>
       <c r="D108" t="n">
-        <v>319.8108303713097</v>
+        <v>319.8108607588288</v>
       </c>
       <c r="E108" t="n">
-        <v>328.4636207960852</v>
+        <v>328.4636520057679</v>
       </c>
       <c r="F108" t="n">
         <v>1069100</v>
@@ -2601,16 +2601,16 @@
         <v>45089</v>
       </c>
       <c r="B109" t="n">
-        <v>330.1746215820312</v>
+        <v>330.1746520996094</v>
       </c>
       <c r="C109" t="n">
-        <v>333.3521977779235</v>
+        <v>333.3522285892006</v>
       </c>
       <c r="D109" t="n">
-        <v>321.1796247232679</v>
+        <v>321.179654409451</v>
       </c>
       <c r="E109" t="n">
-        <v>321.1796247232679</v>
+        <v>321.179654409451</v>
       </c>
       <c r="F109" t="n">
         <v>3123973</v>
@@ -2621,16 +2621,16 @@
         <v>45090</v>
       </c>
       <c r="B110" t="n">
-        <v>328.4147338867188</v>
+        <v>328.4147644042969</v>
       </c>
       <c r="C110" t="n">
-        <v>334.8676641859815</v>
+        <v>334.8676953031911</v>
       </c>
       <c r="D110" t="n">
-        <v>327.5347956271644</v>
+        <v>327.5348260629752</v>
       </c>
       <c r="E110" t="n">
-        <v>331.88564290707</v>
+        <v>331.8856737471785</v>
       </c>
       <c r="F110" t="n">
         <v>1540537</v>
@@ -2641,16 +2641,16 @@
         <v>45091</v>
       </c>
       <c r="B111" t="n">
-        <v>330.7123413085938</v>
+        <v>330.7123718261719</v>
       </c>
       <c r="C111" t="n">
-        <v>332.3744699626676</v>
+        <v>332.3745006336242</v>
       </c>
       <c r="D111" t="n">
-        <v>326.0681916523755</v>
+        <v>326.0682217413993</v>
       </c>
       <c r="E111" t="n">
-        <v>329.4901966622205</v>
+        <v>329.4902270670212</v>
       </c>
       <c r="F111" t="n">
         <v>1179052</v>
@@ -2661,16 +2661,16 @@
         <v>45092</v>
       </c>
       <c r="B112" t="n">
-        <v>327.4859619140625</v>
+        <v>327.4859313964844</v>
       </c>
       <c r="C112" t="n">
-        <v>332.6189705344239</v>
+        <v>332.6189395385138</v>
       </c>
       <c r="D112" t="n">
-        <v>326.7526749682966</v>
+        <v>326.7526445190516</v>
       </c>
       <c r="E112" t="n">
-        <v>329.9302517332822</v>
+        <v>329.9302209879269</v>
       </c>
       <c r="F112" t="n">
         <v>1135497</v>
@@ -2701,16 +2701,16 @@
         <v>45096</v>
       </c>
       <c r="B114" t="n">
-        <v>327.8770446777344</v>
+        <v>327.8770141601562</v>
       </c>
       <c r="C114" t="n">
-        <v>333.4011337414295</v>
+        <v>333.4011027096897</v>
       </c>
       <c r="D114" t="n">
-        <v>326.7037736210547</v>
+        <v>326.7037432126803</v>
       </c>
       <c r="E114" t="n">
-        <v>332.4234178067039</v>
+        <v>332.4233868659663</v>
       </c>
       <c r="F114" t="n">
         <v>1315878</v>
@@ -2781,16 +2781,16 @@
         <v>45100</v>
       </c>
       <c r="B118" t="n">
-        <v>336.0409545898438</v>
+        <v>336.0409851074219</v>
       </c>
       <c r="C118" t="n">
-        <v>342.2005526016657</v>
+        <v>342.200583678628</v>
       </c>
       <c r="D118" t="n">
-        <v>332.2278388479804</v>
+        <v>332.2278690192702</v>
       </c>
       <c r="E118" t="n">
-        <v>341.2228367370894</v>
+        <v>341.2228677252605</v>
       </c>
       <c r="F118" t="n">
         <v>5871422</v>
@@ -2801,16 +2801,16 @@
         <v>45103</v>
       </c>
       <c r="B119" t="n">
-        <v>332.570068359375</v>
+        <v>332.5700073242188</v>
       </c>
       <c r="C119" t="n">
-        <v>335.0143581897945</v>
+        <v>335.0142967060482</v>
       </c>
       <c r="D119" t="n">
-        <v>327.5837111378147</v>
+        <v>327.5836510177832</v>
       </c>
       <c r="E119" t="n">
-        <v>335.0143581897945</v>
+        <v>335.0142967060482</v>
       </c>
       <c r="F119" t="n">
         <v>1283233</v>
@@ -2821,16 +2821,16 @@
         <v>45104</v>
       </c>
       <c r="B120" t="n">
-        <v>344.987060546875</v>
+        <v>344.9870300292969</v>
       </c>
       <c r="C120" t="n">
-        <v>348.4579400494654</v>
+        <v>348.457909224853</v>
       </c>
       <c r="D120" t="n">
-        <v>332.4234052911607</v>
+        <v>332.4233758849643</v>
       </c>
       <c r="E120" t="n">
-        <v>332.4234052911607</v>
+        <v>332.4233758849643</v>
       </c>
       <c r="F120" t="n">
         <v>6798031</v>
@@ -2841,16 +2841,16 @@
         <v>45105</v>
       </c>
       <c r="B121" t="n">
-        <v>343.9115295410156</v>
+        <v>343.9115905761719</v>
       </c>
       <c r="C121" t="n">
-        <v>348.0668216534515</v>
+        <v>348.0668834260617</v>
       </c>
       <c r="D121" t="n">
-        <v>339.8540149751995</v>
+        <v>339.8540752902547</v>
       </c>
       <c r="E121" t="n">
-        <v>346.2091676177485</v>
+        <v>346.2092290606744</v>
       </c>
       <c r="F121" t="n">
         <v>2091878</v>
@@ -2881,16 +2881,16 @@
         <v>45110</v>
       </c>
       <c r="B123" t="n">
-        <v>346.3558349609375</v>
+        <v>346.3558654785156</v>
       </c>
       <c r="C123" t="n">
-        <v>355.9374382203325</v>
+        <v>355.9374695821503</v>
       </c>
       <c r="D123" t="n">
-        <v>345.6225480838148</v>
+        <v>345.6225785367827</v>
       </c>
       <c r="E123" t="n">
-        <v>352.906542998241</v>
+        <v>352.9065740930052</v>
       </c>
       <c r="F123" t="n">
         <v>1734803</v>
@@ -2901,16 +2901,16 @@
         <v>45111</v>
       </c>
       <c r="B124" t="n">
-        <v>346.0625305175781</v>
+        <v>346.0625</v>
       </c>
       <c r="C124" t="n">
-        <v>349.3378546833068</v>
+        <v>349.3378238768937</v>
       </c>
       <c r="D124" t="n">
-        <v>342.493843862349</v>
+        <v>342.4938136594761</v>
       </c>
       <c r="E124" t="n">
-        <v>346.35583333204</v>
+        <v>346.355802788597</v>
       </c>
       <c r="F124" t="n">
         <v>1341376</v>
@@ -2941,16 +2941,16 @@
         <v>45113</v>
       </c>
       <c r="B126" t="n">
-        <v>345.9158935546875</v>
+        <v>345.9158630371094</v>
       </c>
       <c r="C126" t="n">
-        <v>348.2624357208487</v>
+        <v>348.2624049962526</v>
       </c>
       <c r="D126" t="n">
-        <v>341.7117268757745</v>
+        <v>341.7116967290986</v>
       </c>
       <c r="E126" t="n">
-        <v>347.040290774941</v>
+        <v>347.0402601581657</v>
       </c>
       <c r="F126" t="n">
         <v>1989456</v>
@@ -2961,16 +2961,16 @@
         <v>45114</v>
       </c>
       <c r="B127" t="n">
-        <v>346.7958068847656</v>
+        <v>346.7958374023438</v>
       </c>
       <c r="C127" t="n">
-        <v>352.5154204561269</v>
+        <v>352.5154514770236</v>
       </c>
       <c r="D127" t="n">
-        <v>345.1825519415423</v>
+        <v>345.1825823171561</v>
       </c>
       <c r="E127" t="n">
-        <v>348.0668254922863</v>
+        <v>348.0668561217124</v>
       </c>
       <c r="F127" t="n">
         <v>2437598</v>
@@ -2981,16 +2981,16 @@
         <v>45117</v>
       </c>
       <c r="B128" t="n">
-        <v>338.2408142089844</v>
+        <v>338.2407836914062</v>
       </c>
       <c r="C128" t="n">
-        <v>347.7246401626873</v>
+        <v>347.7246087894365</v>
       </c>
       <c r="D128" t="n">
-        <v>335.9431759670365</v>
+        <v>335.9431456567614</v>
       </c>
       <c r="E128" t="n">
-        <v>347.5291148929063</v>
+        <v>347.5290835372967</v>
       </c>
       <c r="F128" t="n">
         <v>1895779</v>
@@ -3041,16 +3041,16 @@
         <v>45120</v>
       </c>
       <c r="B131" t="n">
-        <v>353.8353576660156</v>
+        <v>353.8353271484375</v>
       </c>
       <c r="C131" t="n">
-        <v>358.2839826548289</v>
+        <v>358.283951753566</v>
       </c>
       <c r="D131" t="n">
-        <v>340.3917648227968</v>
+        <v>340.3917354647012</v>
       </c>
       <c r="E131" t="n">
-        <v>341.9072422821805</v>
+        <v>341.9072127933781</v>
       </c>
       <c r="F131" t="n">
         <v>7094935</v>
@@ -3081,16 +3081,16 @@
         <v>45124</v>
       </c>
       <c r="B133" t="n">
-        <v>377.4800720214844</v>
+        <v>377.4801330566406</v>
       </c>
       <c r="C133" t="n">
-        <v>387.01659935663</v>
+        <v>387.0166619337575</v>
       </c>
       <c r="D133" t="n">
-        <v>370.8438162456385</v>
+        <v>370.8438762077714</v>
       </c>
       <c r="E133" t="n">
-        <v>376.7918557174735</v>
+        <v>376.7919166413512</v>
       </c>
       <c r="F133" t="n">
         <v>7245327</v>
@@ -3121,16 +3121,16 @@
         <v>45126</v>
       </c>
       <c r="B135" t="n">
-        <v>386.8691711425781</v>
+        <v>386.869140625</v>
       </c>
       <c r="C135" t="n">
-        <v>391.1950211851837</v>
+        <v>391.1949903263676</v>
       </c>
       <c r="D135" t="n">
-        <v>383.4281492899758</v>
+        <v>383.4281190438373</v>
       </c>
       <c r="E135" t="n">
-        <v>386.8200256888728</v>
+        <v>386.8199951751714</v>
       </c>
       <c r="F135" t="n">
         <v>3453054</v>
@@ -3141,16 +3141,16 @@
         <v>45127</v>
       </c>
       <c r="B136" t="n">
-        <v>385.8368530273438</v>
+        <v>385.8368835449219</v>
       </c>
       <c r="C136" t="n">
-        <v>388.9337665049097</v>
+        <v>388.9337972674367</v>
       </c>
       <c r="D136" t="n">
-        <v>382.9365513559229</v>
+        <v>382.9365816441031</v>
       </c>
       <c r="E136" t="n">
-        <v>386.8691475187565</v>
+        <v>386.8691781179835</v>
       </c>
       <c r="F136" t="n">
         <v>2027313</v>
@@ -3181,16 +3181,16 @@
         <v>45131</v>
       </c>
       <c r="B138" t="n">
-        <v>376.8901977539062</v>
+        <v>376.8902282714844</v>
       </c>
       <c r="C138" t="n">
-        <v>380.0854321955341</v>
+        <v>380.0854629718369</v>
       </c>
       <c r="D138" t="n">
-        <v>373.4491760475378</v>
+        <v>373.4492062864893</v>
       </c>
       <c r="E138" t="n">
-        <v>379.0039622300098</v>
+        <v>379.0039929187438</v>
       </c>
       <c r="F138" t="n">
         <v>2470379</v>
@@ -3221,16 +3221,16 @@
         <v>45133</v>
       </c>
       <c r="B140" t="n">
-        <v>372.908447265625</v>
+        <v>372.9084167480469</v>
       </c>
       <c r="C140" t="n">
-        <v>377.4801146523948</v>
+        <v>377.4800837606867</v>
       </c>
       <c r="D140" t="n">
-        <v>371.6303654176371</v>
+        <v>371.6303350046529</v>
       </c>
       <c r="E140" t="n">
-        <v>372.9576227233661</v>
+        <v>372.9575922017636</v>
       </c>
       <c r="F140" t="n">
         <v>1085762</v>
@@ -3301,16 +3301,16 @@
         <v>45139</v>
       </c>
       <c r="B144" t="n">
-        <v>424.8678588867188</v>
+        <v>424.8678894042969</v>
       </c>
       <c r="C144" t="n">
-        <v>427.5715187928632</v>
+        <v>427.5715495046408</v>
       </c>
       <c r="D144" t="n">
-        <v>412.92260384751</v>
+        <v>412.9226335070796</v>
       </c>
       <c r="E144" t="n">
-        <v>420.7877963017483</v>
+        <v>420.787826526262</v>
       </c>
       <c r="F144" t="n">
         <v>3174123</v>
@@ -3321,16 +3321,16 @@
         <v>45140</v>
       </c>
       <c r="B145" t="n">
-        <v>418.5265808105469</v>
+        <v>418.5265502929688</v>
       </c>
       <c r="C145" t="n">
-        <v>424.5237662740245</v>
+        <v>424.5237353191513</v>
       </c>
       <c r="D145" t="n">
-        <v>411.3495744310364</v>
+        <v>411.3495444367819</v>
       </c>
       <c r="E145" t="n">
-        <v>424.2288335475131</v>
+        <v>424.2288026141456</v>
       </c>
       <c r="F145" t="n">
         <v>2299029</v>
@@ -3421,16 +3421,16 @@
         <v>45147</v>
       </c>
       <c r="B150" t="n">
-        <v>446.4971618652344</v>
+        <v>446.4971313476562</v>
       </c>
       <c r="C150" t="n">
-        <v>447.8735646172102</v>
+        <v>447.8735340055565</v>
       </c>
       <c r="D150" t="n">
-        <v>439.860905379283</v>
+        <v>439.8608753152855</v>
       </c>
       <c r="E150" t="n">
-        <v>443.3511027183367</v>
+        <v>443.3510724157882</v>
       </c>
       <c r="F150" t="n">
         <v>1549021</v>
@@ -3461,16 +3461,16 @@
         <v>45149</v>
       </c>
       <c r="B152" t="n">
-        <v>438.3370056152344</v>
+        <v>438.3370361328125</v>
       </c>
       <c r="C152" t="n">
-        <v>443.5476835274554</v>
+        <v>443.5477144078076</v>
       </c>
       <c r="D152" t="n">
-        <v>433.2737940583917</v>
+        <v>433.2738242234626</v>
       </c>
       <c r="E152" t="n">
-        <v>438.4844719706128</v>
+        <v>438.4845024984577</v>
       </c>
       <c r="F152" t="n">
         <v>1486040</v>
@@ -3521,16 +3521,16 @@
         <v>45155</v>
       </c>
       <c r="B155" t="n">
-        <v>462.1783752441406</v>
+        <v>462.1784057617188</v>
       </c>
       <c r="C155" t="n">
-        <v>464.0463524418639</v>
+        <v>464.0463830827843</v>
       </c>
       <c r="D155" t="n">
-        <v>444.3833714061917</v>
+        <v>444.383400748768</v>
       </c>
       <c r="E155" t="n">
-        <v>445.1698786462874</v>
+        <v>445.1699080407967</v>
       </c>
       <c r="F155" t="n">
         <v>5942124</v>
@@ -3581,16 +3581,16 @@
         <v>45160</v>
       </c>
       <c r="B158" t="n">
-        <v>458.4423828125</v>
+        <v>458.4424133300781</v>
       </c>
       <c r="C158" t="n">
-        <v>461.0477517567375</v>
+        <v>461.0477824477497</v>
       </c>
       <c r="D158" t="n">
-        <v>454.608107578394</v>
+        <v>454.6081378407322</v>
       </c>
       <c r="E158" t="n">
-        <v>456.3777938425927</v>
+        <v>456.3778242227353</v>
       </c>
       <c r="F158" t="n">
         <v>1984953</v>
@@ -3641,16 +3641,16 @@
         <v>45163</v>
       </c>
       <c r="B161" t="n">
-        <v>476.3848876953125</v>
+        <v>476.3848571777344</v>
       </c>
       <c r="C161" t="n">
-        <v>479.4326559270373</v>
+        <v>479.4326252142169</v>
       </c>
       <c r="D161" t="n">
-        <v>468.8146575750027</v>
+        <v>468.8146275423792</v>
       </c>
       <c r="E161" t="n">
-        <v>469.9452730471489</v>
+        <v>469.9452429420974</v>
       </c>
       <c r="F161" t="n">
         <v>3630212</v>
@@ -3661,16 +3661,16 @@
         <v>45166</v>
       </c>
       <c r="B162" t="n">
-        <v>476.8764343261719</v>
+        <v>476.87646484375</v>
       </c>
       <c r="C162" t="n">
-        <v>480.2191650962056</v>
+        <v>480.2191958277009</v>
       </c>
       <c r="D162" t="n">
-        <v>470.2893536983485</v>
+        <v>470.2893837943881</v>
       </c>
       <c r="E162" t="n">
-        <v>477.2205424940669</v>
+        <v>477.2205730336661</v>
       </c>
       <c r="F162" t="n">
         <v>1287199</v>
@@ -3721,16 +3721,16 @@
         <v>45169</v>
       </c>
       <c r="B165" t="n">
-        <v>501.1111145019531</v>
+        <v>501.111083984375</v>
       </c>
       <c r="C165" t="n">
-        <v>503.2740245468482</v>
+        <v>503.2739938975492</v>
       </c>
       <c r="D165" t="n">
-        <v>485.2332323368701</v>
+        <v>485.2332027862522</v>
       </c>
       <c r="E165" t="n">
-        <v>485.6756614387029</v>
+        <v>485.6756318611411</v>
       </c>
       <c r="F165" t="n">
         <v>4221568</v>
@@ -3741,16 +3741,16 @@
         <v>45170</v>
       </c>
       <c r="B166" t="n">
-        <v>519.4468383789062</v>
+        <v>519.44677734375</v>
       </c>
       <c r="C166" t="n">
-        <v>521.9539167600727</v>
+        <v>521.9538554303341</v>
       </c>
       <c r="D166" t="n">
-        <v>499.4397768332323</v>
+        <v>499.4397181489117</v>
       </c>
       <c r="E166" t="n">
-        <v>504.2572317541708</v>
+        <v>504.2571725037978</v>
       </c>
       <c r="F166" t="n">
         <v>3248231</v>
@@ -3801,16 +3801,16 @@
         <v>45175</v>
       </c>
       <c r="B169" t="n">
-        <v>509.9594116210938</v>
+        <v>509.95947265625</v>
       </c>
       <c r="C169" t="n">
-        <v>521.8554908291494</v>
+        <v>521.8555532881034</v>
       </c>
       <c r="D169" t="n">
-        <v>507.1082554439625</v>
+        <v>507.1083161378745</v>
       </c>
       <c r="E169" t="n">
-        <v>515.6125185187487</v>
+        <v>515.6125802305045</v>
       </c>
       <c r="F169" t="n">
         <v>2392443</v>
@@ -3821,16 +3821,16 @@
         <v>45176</v>
       </c>
       <c r="B170" t="n">
-        <v>504.2080078125</v>
+        <v>504.2079772949219</v>
       </c>
       <c r="C170" t="n">
-        <v>515.5142228185922</v>
+        <v>515.5141916166967</v>
       </c>
       <c r="D170" t="n">
-        <v>501.1602695091742</v>
+        <v>501.1602391760628</v>
       </c>
       <c r="E170" t="n">
-        <v>512.1224063220932</v>
+        <v>512.12237532549</v>
       </c>
       <c r="F170" t="n">
         <v>3104273</v>
@@ -3881,16 +3881,16 @@
         <v>45181</v>
       </c>
       <c r="B173" t="n">
-        <v>488.7725524902344</v>
+        <v>488.7725830078125</v>
       </c>
       <c r="C173" t="n">
-        <v>510.8934364934527</v>
+        <v>510.8934683921963</v>
       </c>
       <c r="D173" t="n">
-        <v>486.1180680122447</v>
+        <v>486.1180983640842</v>
       </c>
       <c r="E173" t="n">
-        <v>503.8147512121566</v>
+        <v>503.8147826689271</v>
       </c>
       <c r="F173" t="n">
         <v>3948677</v>
@@ -3901,16 +3901,16 @@
         <v>45182</v>
       </c>
       <c r="B174" t="n">
-        <v>485.7739868164062</v>
+        <v>485.7739562988281</v>
       </c>
       <c r="C174" t="n">
-        <v>493.8357916087597</v>
+        <v>493.8357605847181</v>
       </c>
       <c r="D174" t="n">
-        <v>480.7599202973021</v>
+        <v>480.7598900947206</v>
       </c>
       <c r="E174" t="n">
-        <v>489.6082623886635</v>
+        <v>489.6082316302063</v>
       </c>
       <c r="F174" t="n">
         <v>1815178</v>
@@ -3921,16 +3921,16 @@
         <v>45183</v>
       </c>
       <c r="B175" t="n">
-        <v>497.2276611328125</v>
+        <v>497.2276306152344</v>
       </c>
       <c r="C175" t="n">
-        <v>505.3386412699271</v>
+        <v>505.3386102545338</v>
       </c>
       <c r="D175" t="n">
-        <v>487.9368900653312</v>
+        <v>487.9368601179784</v>
       </c>
       <c r="E175" t="n">
-        <v>489.0675355416533</v>
+        <v>489.0675055249067</v>
       </c>
       <c r="F175" t="n">
         <v>3601415</v>
@@ -4001,16 +4001,16 @@
         <v>45190</v>
       </c>
       <c r="B179" t="n">
-        <v>483.0211181640625</v>
+        <v>483.0211486816406</v>
       </c>
       <c r="C179" t="n">
-        <v>487.2978225490543</v>
+        <v>487.2978533368373</v>
       </c>
       <c r="D179" t="n">
-        <v>470.633464087987</v>
+        <v>470.6334938229053</v>
       </c>
       <c r="E179" t="n">
-        <v>472.8946949105524</v>
+        <v>472.8947247883367</v>
       </c>
       <c r="F179" t="n">
         <v>2815870</v>
@@ -4041,16 +4041,16 @@
         <v>45194</v>
       </c>
       <c r="B181" t="n">
-        <v>480.1700134277344</v>
+        <v>480.1699829101562</v>
       </c>
       <c r="C181" t="n">
-        <v>488.0352062111644</v>
+        <v>488.0351751937078</v>
       </c>
       <c r="D181" t="n">
-        <v>476.8273124954425</v>
+        <v>476.8272821903123</v>
       </c>
       <c r="E181" t="n">
-        <v>481.5464161641688</v>
+        <v>481.5463855591123</v>
       </c>
       <c r="F181" t="n">
         <v>1287496</v>
@@ -4061,16 +4061,16 @@
         <v>45195</v>
       </c>
       <c r="B182" t="n">
-        <v>475.598388671875</v>
+        <v>475.5983581542969</v>
       </c>
       <c r="C182" t="n">
-        <v>484.1517980508718</v>
+        <v>484.1517669844497</v>
       </c>
       <c r="D182" t="n">
-        <v>474.8118813741115</v>
+        <v>474.8118509070009</v>
       </c>
       <c r="E182" t="n">
-        <v>481.2023506792632</v>
+        <v>481.2023198020975</v>
       </c>
       <c r="F182" t="n">
         <v>931591</v>
@@ -4121,16 +4121,16 @@
         <v>45198</v>
       </c>
       <c r="B185" t="n">
-        <v>475.2051086425781</v>
+        <v>475.205078125</v>
       </c>
       <c r="C185" t="n">
-        <v>481.1531485104586</v>
+        <v>481.1531176108986</v>
       </c>
       <c r="D185" t="n">
-        <v>467.978956982622</v>
+        <v>467.9789269291059</v>
       </c>
       <c r="E185" t="n">
-        <v>469.355359678964</v>
+        <v>469.3553295370555</v>
       </c>
       <c r="F185" t="n">
         <v>1618689</v>
@@ -4161,16 +4161,16 @@
         <v>45203</v>
       </c>
       <c r="B187" t="n">
-        <v>483.1194458007812</v>
+        <v>483.1194152832031</v>
       </c>
       <c r="C187" t="n">
-        <v>489.3624483804848</v>
+        <v>489.3624174685501</v>
       </c>
       <c r="D187" t="n">
-        <v>471.9115524312058</v>
+        <v>471.9115226216053</v>
       </c>
       <c r="E187" t="n">
-        <v>487.5927920601991</v>
+        <v>487.5927612600497</v>
       </c>
       <c r="F187" t="n">
         <v>1785367</v>
@@ -4201,16 +4201,16 @@
         <v>45205</v>
       </c>
       <c r="B189" t="n">
-        <v>504.0605163574219</v>
+        <v>504.060546875</v>
       </c>
       <c r="C189" t="n">
-        <v>511.7290667395073</v>
+        <v>511.7290977213661</v>
       </c>
       <c r="D189" t="n">
-        <v>500.7669611279815</v>
+        <v>500.7669914461563</v>
       </c>
       <c r="E189" t="n">
-        <v>507.2557506838453</v>
+        <v>507.255781394874</v>
       </c>
       <c r="F189" t="n">
         <v>3080842</v>
@@ -4241,16 +4241,16 @@
         <v>45209</v>
       </c>
       <c r="B191" t="n">
-        <v>530.0156860351562</v>
+        <v>530.015625</v>
       </c>
       <c r="C191" t="n">
-        <v>534.5382081570798</v>
+        <v>534.5381466011223</v>
       </c>
       <c r="D191" t="n">
-        <v>506.9608863306236</v>
+        <v>506.960827950395</v>
       </c>
       <c r="E191" t="n">
-        <v>508.1406173125787</v>
+        <v>508.1405587964956</v>
       </c>
       <c r="F191" t="n">
         <v>6462169</v>
@@ -4281,16 +4281,16 @@
         <v>45211</v>
       </c>
       <c r="B193" t="n">
-        <v>534.5872802734375</v>
+        <v>534.5873413085938</v>
       </c>
       <c r="C193" t="n">
-        <v>539.6013162788578</v>
+        <v>539.601377886479</v>
       </c>
       <c r="D193" t="n">
-        <v>531.8836204651581</v>
+        <v>531.8836811916308</v>
       </c>
       <c r="E193" t="n">
-        <v>533.8499185075432</v>
+        <v>533.849979458513</v>
       </c>
       <c r="F193" t="n">
         <v>3194908</v>
@@ -4321,16 +4321,16 @@
         <v>45215</v>
       </c>
       <c r="B195" t="n">
-        <v>534.9313354492188</v>
+        <v>534.931396484375</v>
       </c>
       <c r="C195" t="n">
-        <v>538.6673495745862</v>
+        <v>538.6674110360181</v>
       </c>
       <c r="D195" t="n">
-        <v>531.0970904352675</v>
+        <v>531.09715103294</v>
       </c>
       <c r="E195" t="n">
-        <v>532.3751721065846</v>
+        <v>532.375232850085</v>
       </c>
       <c r="F195" t="n">
         <v>1073524</v>
@@ -4421,16 +4421,16 @@
         <v>45222</v>
       </c>
       <c r="B200" t="n">
-        <v>517.5787963867188</v>
+        <v>517.578857421875</v>
       </c>
       <c r="C200" t="n">
-        <v>539.0114323094106</v>
+        <v>539.011495871997</v>
       </c>
       <c r="D200" t="n">
-        <v>514.0394240283018</v>
+        <v>514.0394846460798</v>
       </c>
       <c r="E200" t="n">
-        <v>537.6842051791617</v>
+        <v>537.6842685852357</v>
       </c>
       <c r="F200" t="n">
         <v>1728468</v>
@@ -4481,16 +4481,16 @@
         <v>45226</v>
       </c>
       <c r="B203" t="n">
-        <v>533.2600708007812</v>
+        <v>533.2601318359375</v>
       </c>
       <c r="C203" t="n">
-        <v>534.2923653059729</v>
+        <v>534.2924264592822</v>
       </c>
       <c r="D203" t="n">
-        <v>520.0858494767789</v>
+        <v>520.085909004058</v>
       </c>
       <c r="E203" t="n">
-        <v>525.9355983484065</v>
+        <v>525.9356585452283</v>
       </c>
       <c r="F203" t="n">
         <v>1436568</v>
@@ -4501,16 +4501,16 @@
         <v>45229</v>
       </c>
       <c r="B204" t="n">
-        <v>532.9158935546875</v>
+        <v>532.9159545898438</v>
       </c>
       <c r="C204" t="n">
-        <v>535.7179041566577</v>
+        <v>535.7179655127298</v>
       </c>
       <c r="D204" t="n">
-        <v>527.5085741550785</v>
+        <v>527.5086345709313</v>
       </c>
       <c r="E204" t="n">
-        <v>534.8330460704246</v>
+        <v>534.8331073251535</v>
       </c>
       <c r="F204" t="n">
         <v>823028</v>
@@ -4521,16 +4521,16 @@
         <v>45230</v>
       </c>
       <c r="B205" t="n">
-        <v>538.4216918945312</v>
+        <v>538.421630859375</v>
       </c>
       <c r="C205" t="n">
-        <v>542.6983669794748</v>
+        <v>542.6983054595173</v>
       </c>
       <c r="D205" t="n">
-        <v>530.9005763929645</v>
+        <v>530.9005162103973</v>
       </c>
       <c r="E205" t="n">
-        <v>536.9961135306614</v>
+        <v>536.9960526571078</v>
       </c>
       <c r="F205" t="n">
         <v>1369699</v>
@@ -4541,16 +4541,16 @@
         <v>45231</v>
       </c>
       <c r="B206" t="n">
-        <v>564.524169921875</v>
+        <v>564.5242309570312</v>
       </c>
       <c r="C206" t="n">
-        <v>573.4708018528205</v>
+        <v>573.4708638552676</v>
       </c>
       <c r="D206" t="n">
-        <v>535.0296998110838</v>
+        <v>535.0297576573604</v>
       </c>
       <c r="E206" t="n">
-        <v>551.9890201247888</v>
+        <v>551.9890798046712</v>
       </c>
       <c r="F206" t="n">
         <v>13001342</v>
@@ -4561,16 +4561,16 @@
         <v>45232</v>
       </c>
       <c r="B207" t="n">
-        <v>567.9652709960938</v>
+        <v>567.9652099609375</v>
       </c>
       <c r="C207" t="n">
-        <v>575.5355313863124</v>
+        <v>575.5354695376345</v>
       </c>
       <c r="D207" t="n">
-        <v>566.5396927397114</v>
+        <v>566.5396318577518</v>
       </c>
       <c r="E207" t="n">
-        <v>569.4891401639529</v>
+        <v>569.4890789650373</v>
       </c>
       <c r="F207" t="n">
         <v>3252737</v>
@@ -4581,16 +4581,16 @@
         <v>45233</v>
       </c>
       <c r="B208" t="n">
-        <v>577.8458862304688</v>
+        <v>577.8458251953125</v>
       </c>
       <c r="C208" t="n">
-        <v>583.007419029635</v>
+        <v>583.0073574492902</v>
       </c>
       <c r="D208" t="n">
-        <v>569.2433315651917</v>
+        <v>569.243271438683</v>
       </c>
       <c r="E208" t="n">
-        <v>570.2264806697948</v>
+        <v>570.2264204394406</v>
       </c>
       <c r="F208" t="n">
         <v>3063927</v>
@@ -4681,16 +4681,16 @@
         <v>45240</v>
       </c>
       <c r="B213" t="n">
-        <v>577.52587890625</v>
+        <v>577.5258178710938</v>
       </c>
       <c r="C213" t="n">
-        <v>587.9201563741093</v>
+        <v>587.9200942404458</v>
       </c>
       <c r="D213" t="n">
-        <v>574.1600887007966</v>
+        <v>574.1600280213499</v>
       </c>
       <c r="E213" t="n">
-        <v>578.7137479946645</v>
+        <v>578.7136868339696</v>
       </c>
       <c r="F213" t="n">
         <v>2069707</v>
@@ -4701,16 +4701,16 @@
         <v>45243</v>
       </c>
       <c r="B214" t="n">
-        <v>577.3773193359375</v>
+        <v>577.3773803710938</v>
       </c>
       <c r="C214" t="n">
-        <v>587.0291476488828</v>
+        <v>587.029209704344</v>
       </c>
       <c r="D214" t="n">
-        <v>575.7934537297454</v>
+        <v>575.7935145974697</v>
       </c>
       <c r="E214" t="n">
-        <v>586.0392165398629</v>
+        <v>586.0392784906772</v>
       </c>
       <c r="F214" t="n">
         <v>806673</v>
@@ -4841,16 +4841,16 @@
         <v>45253</v>
       </c>
       <c r="B221" t="n">
-        <v>615.9352416992188</v>
+        <v>615.9351806640625</v>
       </c>
       <c r="C221" t="n">
-        <v>625.0426213700633</v>
+        <v>625.0425594324253</v>
       </c>
       <c r="D221" t="n">
-        <v>611.9260321826637</v>
+        <v>611.9259715447939</v>
       </c>
       <c r="E221" t="n">
-        <v>620.7858686180425</v>
+        <v>620.7858071022209</v>
       </c>
       <c r="F221" t="n">
         <v>851855</v>
@@ -4881,16 +4881,16 @@
         <v>45258</v>
       </c>
       <c r="B223" t="n">
-        <v>605.5408935546875</v>
+        <v>605.5409545898438</v>
       </c>
       <c r="C223" t="n">
-        <v>612.1238994173815</v>
+        <v>612.1239611160681</v>
       </c>
       <c r="D223" t="n">
-        <v>594.0576560189216</v>
+        <v>594.0577158966314</v>
       </c>
       <c r="E223" t="n">
-        <v>611.7774476848299</v>
+        <v>611.7775093485961</v>
       </c>
       <c r="F223" t="n">
         <v>1833462</v>
@@ -5001,16 +5001,16 @@
         <v>45266</v>
       </c>
       <c r="B229" t="n">
-        <v>646.771484375</v>
+        <v>646.7715454101562</v>
       </c>
       <c r="C229" t="n">
-        <v>653.2060367673334</v>
+        <v>653.2060984097118</v>
       </c>
       <c r="D229" t="n">
-        <v>633.6054123332689</v>
+        <v>633.6054721259565</v>
       </c>
       <c r="E229" t="n">
-        <v>636.3277229607945</v>
+        <v>636.3277830103838</v>
       </c>
       <c r="F229" t="n">
         <v>3523055</v>
@@ -5081,16 +5081,16 @@
         <v>45272</v>
       </c>
       <c r="B233" t="n">
-        <v>657.2647705078125</v>
+        <v>657.2648315429688</v>
       </c>
       <c r="C233" t="n">
-        <v>663.055843314915</v>
+        <v>663.0559048878439</v>
       </c>
       <c r="D233" t="n">
-        <v>653.9980099391752</v>
+        <v>653.9980706709723</v>
       </c>
       <c r="E233" t="n">
-        <v>654.4929754926233</v>
+        <v>654.4930362703841</v>
       </c>
       <c r="F233" t="n">
         <v>1566679</v>
@@ -5121,16 +5121,16 @@
         <v>45274</v>
       </c>
       <c r="B235" t="n">
-        <v>693.3477783203125</v>
+        <v>693.3478393554688</v>
       </c>
       <c r="C235" t="n">
-        <v>699.8812995224374</v>
+        <v>699.8813611327372</v>
       </c>
       <c r="D235" t="n">
-        <v>671.3218109732485</v>
+        <v>671.3218700694667</v>
       </c>
       <c r="E235" t="n">
-        <v>673.1531593709441</v>
+        <v>673.1532186283753</v>
       </c>
       <c r="F235" t="n">
         <v>4534231</v>
@@ -5141,16 +5141,16 @@
         <v>45275</v>
       </c>
       <c r="B236" t="n">
-        <v>712.3544311523438</v>
+        <v>712.3544921875</v>
       </c>
       <c r="C236" t="n">
-        <v>723.689154900473</v>
+        <v>723.6892169067984</v>
       </c>
       <c r="D236" t="n">
-        <v>691.9618736368659</v>
+        <v>691.9619329247698</v>
       </c>
       <c r="E236" t="n">
-        <v>697.1095276994008</v>
+        <v>697.1095874283603</v>
       </c>
       <c r="F236" t="n">
         <v>5448159</v>
@@ -5161,16 +5161,16 @@
         <v>45278</v>
       </c>
       <c r="B237" t="n">
-        <v>709.2361450195312</v>
+        <v>709.2362060546875</v>
       </c>
       <c r="C237" t="n">
-        <v>720.1253870633439</v>
+        <v>720.1254490356021</v>
       </c>
       <c r="D237" t="n">
-        <v>698.6933546906913</v>
+        <v>698.6934148185603</v>
       </c>
       <c r="E237" t="n">
-        <v>711.6614882861365</v>
+        <v>711.6615495300121</v>
       </c>
       <c r="F237" t="n">
         <v>2558759</v>
@@ -5261,16 +5261,16 @@
         <v>45286</v>
       </c>
       <c r="B242" t="n">
-        <v>727.302490234375</v>
+        <v>727.3024291992188</v>
       </c>
       <c r="C242" t="n">
-        <v>738.488701102612</v>
+        <v>738.4886391287101</v>
       </c>
       <c r="D242" t="n">
-        <v>722.6003168694455</v>
+        <v>722.6002562288952</v>
       </c>
       <c r="E242" t="n">
-        <v>734.9249728258559</v>
+        <v>734.9249111510217</v>
       </c>
       <c r="F242" t="n">
         <v>1544968</v>
@@ -5281,16 +5281,16 @@
         <v>45287</v>
       </c>
       <c r="B243" t="n">
-        <v>727.599365234375</v>
+        <v>727.5994262695312</v>
       </c>
       <c r="C243" t="n">
-        <v>735.766296884965</v>
+        <v>735.7663586052096</v>
       </c>
       <c r="D243" t="n">
-        <v>719.2839197491708</v>
+        <v>719.2839800867803</v>
       </c>
       <c r="E243" t="n">
-        <v>730.5691585618623</v>
+        <v>730.5692198461416</v>
       </c>
       <c r="F243" t="n">
         <v>990093</v>

</xml_diff>

<commit_message>
feat: reconfigured model training logic
</commit_message>
<xml_diff>
--- a/src/data/raw/BSOFT.NS_data.xlsx
+++ b/src/data/raw/BSOFT.NS_data.xlsx
@@ -481,16 +481,16 @@
         <v>44930</v>
       </c>
       <c r="B3" t="n">
-        <v>288.1817626953125</v>
+        <v>288.1817016601562</v>
       </c>
       <c r="C3" t="n">
-        <v>293.2169936332564</v>
+        <v>293.2169315316686</v>
       </c>
       <c r="D3" t="n">
-        <v>286.1285533294701</v>
+        <v>286.1284927291712</v>
       </c>
       <c r="E3" t="n">
-        <v>293.2169936332564</v>
+        <v>293.2169315316686</v>
       </c>
       <c r="F3" t="n">
         <v>1599439</v>
@@ -521,16 +521,16 @@
         <v>44932</v>
       </c>
       <c r="B5" t="n">
-        <v>277.3290710449219</v>
+        <v>277.3291015625</v>
       </c>
       <c r="C5" t="n">
-        <v>285.0041457751524</v>
+        <v>285.0041771373037</v>
       </c>
       <c r="D5" t="n">
-        <v>276.4491328230681</v>
+        <v>276.4491632438169</v>
       </c>
       <c r="E5" t="n">
-        <v>284.4175103480775</v>
+        <v>284.4175416456748</v>
       </c>
       <c r="F5" t="n">
         <v>2295178</v>
@@ -541,16 +541,16 @@
         <v>44935</v>
       </c>
       <c r="B6" t="n">
-        <v>287.1062316894531</v>
+        <v>287.1062622070312</v>
       </c>
       <c r="C6" t="n">
-        <v>288.3772801009167</v>
+        <v>288.3773107535992</v>
       </c>
       <c r="D6" t="n">
-        <v>280.9955080887176</v>
+        <v>280.9955379567645</v>
       </c>
       <c r="E6" t="n">
-        <v>280.9955080887176</v>
+        <v>280.9955379567645</v>
       </c>
       <c r="F6" t="n">
         <v>3174952</v>
@@ -561,16 +561,16 @@
         <v>44936</v>
       </c>
       <c r="B7" t="n">
-        <v>283.8798217773438</v>
+        <v>283.8797912597656</v>
       </c>
       <c r="C7" t="n">
-        <v>286.9107470801693</v>
+        <v>286.9107162367614</v>
       </c>
       <c r="D7" t="n">
-        <v>281.582183410483</v>
+        <v>281.582153139905</v>
       </c>
       <c r="E7" t="n">
-        <v>286.9107470801693</v>
+        <v>286.9107162367614</v>
       </c>
       <c r="F7" t="n">
         <v>1398351</v>
@@ -581,16 +581,16 @@
         <v>44937</v>
       </c>
       <c r="B8" t="n">
-        <v>287.7417297363281</v>
+        <v>287.7417907714844</v>
       </c>
       <c r="C8" t="n">
-        <v>291.3104160497676</v>
+        <v>291.3104778419059</v>
       </c>
       <c r="D8" t="n">
-        <v>284.0264218672196</v>
+        <v>284.0264821142928</v>
       </c>
       <c r="E8" t="n">
-        <v>285.3463440809217</v>
+        <v>285.3464046079739</v>
       </c>
       <c r="F8" t="n">
         <v>1536020</v>
@@ -661,16 +661,16 @@
         <v>44943</v>
       </c>
       <c r="B12" t="n">
-        <v>289.6483459472656</v>
+        <v>289.6483154296875</v>
       </c>
       <c r="C12" t="n">
-        <v>292.8259227382483</v>
+        <v>292.8258918858781</v>
       </c>
       <c r="D12" t="n">
-        <v>288.4262010276569</v>
+        <v>288.426170638845</v>
       </c>
       <c r="E12" t="n">
-        <v>290.3816328990309</v>
+        <v>290.3816023041931</v>
       </c>
       <c r="F12" t="n">
         <v>1047676</v>
@@ -681,16 +681,16 @@
         <v>44944</v>
       </c>
       <c r="B13" t="n">
-        <v>288.1817626953125</v>
+        <v>288.1817016601562</v>
       </c>
       <c r="C13" t="n">
-        <v>292.2392777292859</v>
+        <v>292.2392158347724</v>
       </c>
       <c r="D13" t="n">
-        <v>287.546253325236</v>
+        <v>287.5461924246767</v>
       </c>
       <c r="E13" t="n">
-        <v>290.3816234792462</v>
+        <v>290.3815619781727</v>
       </c>
       <c r="F13" t="n">
         <v>1004351</v>
@@ -701,16 +701,16 @@
         <v>44945</v>
       </c>
       <c r="B14" t="n">
-        <v>288.2306213378906</v>
+        <v>288.2305908203125</v>
       </c>
       <c r="C14" t="n">
-        <v>289.0616857798925</v>
+        <v>289.061655174322</v>
       </c>
       <c r="D14" t="n">
-        <v>283.9286775550528</v>
+        <v>283.9286474929604</v>
       </c>
       <c r="E14" t="n">
-        <v>286.5196185962774</v>
+        <v>286.5195882598586</v>
       </c>
       <c r="F14" t="n">
         <v>755390</v>
@@ -781,16 +781,16 @@
         <v>44951</v>
       </c>
       <c r="B18" t="n">
-        <v>289.3550415039062</v>
+        <v>289.3550109863281</v>
       </c>
       <c r="C18" t="n">
-        <v>299.1810746682973</v>
+        <v>299.1810431143912</v>
       </c>
       <c r="D18" t="n">
-        <v>288.3284218745899</v>
+        <v>288.3283914652869</v>
       </c>
       <c r="E18" t="n">
-        <v>299.1810746682973</v>
+        <v>299.1810431143912</v>
       </c>
       <c r="F18" t="n">
         <v>1965674</v>
@@ -821,16 +821,16 @@
         <v>44956</v>
       </c>
       <c r="B20" t="n">
-        <v>288.2306213378906</v>
+        <v>288.2305908203125</v>
       </c>
       <c r="C20" t="n">
-        <v>292.3370398527703</v>
+        <v>292.3370089004085</v>
       </c>
       <c r="D20" t="n">
-        <v>280.6044496245655</v>
+        <v>280.6044199144389</v>
       </c>
       <c r="E20" t="n">
-        <v>284.5641868915766</v>
+        <v>284.564156762197</v>
       </c>
       <c r="F20" t="n">
         <v>1560058</v>
@@ -861,16 +861,16 @@
         <v>44958</v>
       </c>
       <c r="B22" t="n">
-        <v>289.4039306640625</v>
+        <v>289.4038696289062</v>
       </c>
       <c r="C22" t="n">
-        <v>298.936661488301</v>
+        <v>298.9365984426962</v>
       </c>
       <c r="D22" t="n">
-        <v>284.6620021839878</v>
+        <v>284.6619421489021</v>
       </c>
       <c r="E22" t="n">
-        <v>296.9323556602656</v>
+        <v>296.9322930373679</v>
       </c>
       <c r="F22" t="n">
         <v>1939798</v>
@@ -881,16 +881,16 @@
         <v>44959</v>
       </c>
       <c r="B23" t="n">
-        <v>265.9386901855469</v>
+        <v>265.938720703125</v>
       </c>
       <c r="C23" t="n">
-        <v>288.4261529585895</v>
+        <v>288.4261860566981</v>
       </c>
       <c r="D23" t="n">
-        <v>262.2233821841381</v>
+        <v>262.2234122753691</v>
       </c>
       <c r="E23" t="n">
-        <v>288.4261529585895</v>
+        <v>288.4261860566981</v>
       </c>
       <c r="F23" t="n">
         <v>9755632</v>
@@ -941,16 +941,16 @@
         <v>44964</v>
       </c>
       <c r="B26" t="n">
-        <v>271.5116882324219</v>
+        <v>271.51171875</v>
       </c>
       <c r="C26" t="n">
-        <v>279.5289398496762</v>
+        <v>279.5289712683835</v>
       </c>
       <c r="D26" t="n">
-        <v>270.1917659415423</v>
+        <v>270.1917963107628</v>
       </c>
       <c r="E26" t="n">
-        <v>277.4757307124766</v>
+        <v>277.4757619004057</v>
       </c>
       <c r="F26" t="n">
         <v>1559908</v>
@@ -981,16 +981,16 @@
         <v>44966</v>
       </c>
       <c r="B28" t="n">
-        <v>281.87548828125</v>
+        <v>281.8754577636719</v>
       </c>
       <c r="C28" t="n">
-        <v>282.7554564807669</v>
+        <v>282.7554258679179</v>
       </c>
       <c r="D28" t="n">
-        <v>277.4757666337538</v>
+        <v>277.4757365925166</v>
       </c>
       <c r="E28" t="n">
-        <v>281.0444536178517</v>
+        <v>281.0444231902464</v>
       </c>
       <c r="F28" t="n">
         <v>1510346</v>
@@ -1001,16 +1001,16 @@
         <v>44967</v>
       </c>
       <c r="B29" t="n">
-        <v>285.9329833984375</v>
+        <v>285.9330139160156</v>
       </c>
       <c r="C29" t="n">
-        <v>286.6662702119016</v>
+        <v>286.6663008077433</v>
       </c>
       <c r="D29" t="n">
-        <v>277.182415489426</v>
+        <v>277.1824450730575</v>
       </c>
       <c r="E29" t="n">
-        <v>279.8222599529034</v>
+        <v>279.8222898182851</v>
       </c>
       <c r="F29" t="n">
         <v>1732448</v>
@@ -1021,16 +1021,16 @@
         <v>44970</v>
       </c>
       <c r="B30" t="n">
-        <v>281.1421508789062</v>
+        <v>281.1421813964844</v>
       </c>
       <c r="C30" t="n">
-        <v>284.8085849270793</v>
+        <v>284.8086158426436</v>
       </c>
       <c r="D30" t="n">
-        <v>276.7913337109175</v>
+        <v>276.7913637562207</v>
       </c>
       <c r="E30" t="n">
-        <v>284.0264242651424</v>
+        <v>284.0264550958043</v>
       </c>
       <c r="F30" t="n">
         <v>3345334</v>
@@ -1041,16 +1041,16 @@
         <v>44971</v>
       </c>
       <c r="B31" t="n">
-        <v>281.3866271972656</v>
+        <v>281.3865966796875</v>
       </c>
       <c r="C31" t="n">
-        <v>288.3284161315495</v>
+        <v>288.3283848611048</v>
       </c>
       <c r="D31" t="n">
-        <v>280.6044664036231</v>
+        <v>280.6044359708736</v>
       </c>
       <c r="E31" t="n">
-        <v>282.5598982252511</v>
+        <v>282.5598675804268</v>
       </c>
       <c r="F31" t="n">
         <v>1826849</v>
@@ -1061,16 +1061,16 @@
         <v>44972</v>
       </c>
       <c r="B32" t="n">
-        <v>286.5196228027344</v>
+        <v>286.5195922851562</v>
       </c>
       <c r="C32" t="n">
-        <v>289.0616900236701</v>
+        <v>289.061659235333</v>
       </c>
       <c r="D32" t="n">
-        <v>278.1601640774194</v>
+        <v>278.160134450218</v>
       </c>
       <c r="E32" t="n">
-        <v>280.1155958108283</v>
+        <v>280.1155659753514</v>
       </c>
       <c r="F32" t="n">
         <v>1518654</v>
@@ -1081,16 +1081,16 @@
         <v>44973</v>
       </c>
       <c r="B33" t="n">
-        <v>289.0616760253906</v>
+        <v>289.0617065429688</v>
       </c>
       <c r="C33" t="n">
-        <v>292.8258878974188</v>
+        <v>292.8259188124022</v>
       </c>
       <c r="D33" t="n">
-        <v>287.7906573952341</v>
+        <v>287.7906877786249</v>
       </c>
       <c r="E33" t="n">
-        <v>287.9861826565942</v>
+        <v>287.9862130606275</v>
       </c>
       <c r="F33" t="n">
         <v>2210344</v>
@@ -1121,16 +1121,16 @@
         <v>44977</v>
       </c>
       <c r="B35" t="n">
-        <v>284.9063720703125</v>
+        <v>284.9064025878906</v>
       </c>
       <c r="C35" t="n">
-        <v>289.6971734205347</v>
+        <v>289.6972044512768</v>
       </c>
       <c r="D35" t="n">
-        <v>282.5598601679095</v>
+        <v>282.5598904341424</v>
       </c>
       <c r="E35" t="n">
-        <v>283.5375759470372</v>
+        <v>283.5376063179976</v>
       </c>
       <c r="F35" t="n">
         <v>1101333</v>
@@ -1141,16 +1141,16 @@
         <v>44978</v>
       </c>
       <c r="B36" t="n">
-        <v>280.7022399902344</v>
+        <v>280.7022094726562</v>
       </c>
       <c r="C36" t="n">
-        <v>287.4484737118867</v>
+        <v>287.4484424608669</v>
       </c>
       <c r="D36" t="n">
-        <v>279.7733979530956</v>
+        <v>279.7733675365</v>
       </c>
       <c r="E36" t="n">
-        <v>285.0041839694386</v>
+        <v>285.0041529841588</v>
       </c>
       <c r="F36" t="n">
         <v>856874</v>
@@ -1161,16 +1161,16 @@
         <v>44979</v>
       </c>
       <c r="B37" t="n">
-        <v>276.2536010742188</v>
+        <v>276.2536315917969</v>
       </c>
       <c r="C37" t="n">
-        <v>279.6756065441614</v>
+        <v>279.6756374397665</v>
       </c>
       <c r="D37" t="n">
-        <v>274.0048665575501</v>
+        <v>274.0048968267118</v>
       </c>
       <c r="E37" t="n">
-        <v>278.160158913909</v>
+        <v>278.1601896421035</v>
       </c>
       <c r="F37" t="n">
         <v>1501101</v>
@@ -1181,16 +1181,16 @@
         <v>44980</v>
       </c>
       <c r="B38" t="n">
-        <v>276.742431640625</v>
+        <v>276.7424621582031</v>
       </c>
       <c r="C38" t="n">
-        <v>278.844544377226</v>
+        <v>278.8445751266132</v>
       </c>
       <c r="D38" t="n">
-        <v>273.2226788037942</v>
+        <v>273.222708933234</v>
       </c>
       <c r="E38" t="n">
-        <v>277.5246221446561</v>
+        <v>277.5246527484897</v>
       </c>
       <c r="F38" t="n">
         <v>1796972</v>
@@ -1201,16 +1201,16 @@
         <v>44981</v>
       </c>
       <c r="B39" t="n">
-        <v>276.6447143554688</v>
+        <v>276.6446838378906</v>
       </c>
       <c r="C39" t="n">
-        <v>281.0933095807827</v>
+        <v>281.0932785724655</v>
       </c>
       <c r="D39" t="n">
-        <v>275.8625237654276</v>
+        <v>275.8624933341354</v>
       </c>
       <c r="E39" t="n">
-        <v>278.1601620025484</v>
+        <v>278.1601313177963</v>
       </c>
       <c r="F39" t="n">
         <v>629355</v>
@@ -1221,16 +1221,16 @@
         <v>44984</v>
       </c>
       <c r="B40" t="n">
-        <v>271.560546875</v>
+        <v>271.5605773925781</v>
       </c>
       <c r="C40" t="n">
-        <v>278.5512084508135</v>
+        <v>278.551239753992</v>
       </c>
       <c r="D40" t="n">
-        <v>266.2808878447535</v>
+        <v>266.2809177690113</v>
       </c>
       <c r="E40" t="n">
-        <v>276.1069191000034</v>
+        <v>276.1069501284962</v>
       </c>
       <c r="F40" t="n">
         <v>1433566</v>
@@ -1261,16 +1261,16 @@
         <v>44986</v>
       </c>
       <c r="B42" t="n">
-        <v>270.8273010253906</v>
+        <v>270.8272705078125</v>
       </c>
       <c r="C42" t="n">
-        <v>272.8316066611478</v>
+        <v>272.8315759177189</v>
       </c>
       <c r="D42" t="n">
-        <v>268.2363598892223</v>
+        <v>268.2363296635987</v>
       </c>
       <c r="E42" t="n">
-        <v>269.8495851372123</v>
+        <v>269.849554729806</v>
       </c>
       <c r="F42" t="n">
         <v>1276137</v>
@@ -1281,16 +1281,16 @@
         <v>44987</v>
       </c>
       <c r="B43" t="n">
-        <v>270.4361877441406</v>
+        <v>270.4362182617188</v>
       </c>
       <c r="C43" t="n">
-        <v>274.8359087057996</v>
+        <v>274.8359397198676</v>
       </c>
       <c r="D43" t="n">
-        <v>269.4095682839098</v>
+        <v>269.4095986856382</v>
       </c>
       <c r="E43" t="n">
-        <v>269.8495523150826</v>
+        <v>269.8495827664614</v>
       </c>
       <c r="F43" t="n">
         <v>1179640</v>
@@ -1361,16 +1361,16 @@
         <v>44994</v>
       </c>
       <c r="B47" t="n">
-        <v>275.0314636230469</v>
+        <v>275.0314331054688</v>
       </c>
       <c r="C47" t="n">
-        <v>282.706539207084</v>
+        <v>282.706507837877</v>
       </c>
       <c r="D47" t="n">
-        <v>274.3959542719846</v>
+        <v>274.3959238249228</v>
       </c>
       <c r="E47" t="n">
-        <v>280.8000111538971</v>
+        <v>280.7999799962391</v>
       </c>
       <c r="F47" t="n">
         <v>943696</v>
@@ -1421,16 +1421,16 @@
         <v>44999</v>
       </c>
       <c r="B50" t="n">
-        <v>267.8941650390625</v>
+        <v>267.8941345214844</v>
       </c>
       <c r="C50" t="n">
-        <v>272.3427605891913</v>
+        <v>272.3427295648445</v>
       </c>
       <c r="D50" t="n">
-        <v>263.9833013158645</v>
+        <v>263.9832712437985</v>
       </c>
       <c r="E50" t="n">
-        <v>271.5117259180296</v>
+        <v>271.5116949883514</v>
       </c>
       <c r="F50" t="n">
         <v>1505215</v>
@@ -1441,16 +1441,16 @@
         <v>45000</v>
       </c>
       <c r="B51" t="n">
-        <v>268.5296325683594</v>
+        <v>268.5296630859375</v>
       </c>
       <c r="C51" t="n">
-        <v>273.7604179502698</v>
+        <v>273.7604490623108</v>
       </c>
       <c r="D51" t="n">
-        <v>267.3074878453671</v>
+        <v>267.3075182240522</v>
       </c>
       <c r="E51" t="n">
-        <v>271.8049863934822</v>
+        <v>271.8050172832944</v>
       </c>
       <c r="F51" t="n">
         <v>876676</v>
@@ -1461,16 +1461,16 @@
         <v>45001</v>
       </c>
       <c r="B52" t="n">
-        <v>264.8143310546875</v>
+        <v>264.8143005371094</v>
       </c>
       <c r="C52" t="n">
-        <v>270.3872932260068</v>
+        <v>270.3872620661926</v>
       </c>
       <c r="D52" t="n">
-        <v>257.9214167450705</v>
+        <v>257.9213870218416</v>
       </c>
       <c r="E52" t="n">
-        <v>266.280904758327</v>
+        <v>266.2808740717389</v>
       </c>
       <c r="F52" t="n">
         <v>1749445</v>
@@ -1481,16 +1481,16 @@
         <v>45002</v>
       </c>
       <c r="B53" t="n">
-        <v>270.3872680664062</v>
+        <v>270.3873291015625</v>
       </c>
       <c r="C53" t="n">
-        <v>271.6094127057183</v>
+        <v>271.6094740167522</v>
       </c>
       <c r="D53" t="n">
-        <v>267.6985498599196</v>
+        <v>267.6986102881451</v>
       </c>
       <c r="E53" t="n">
-        <v>268.2851852542925</v>
+        <v>268.2852458149407</v>
       </c>
       <c r="F53" t="n">
         <v>907042</v>
@@ -1501,16 +1501,16 @@
         <v>45005</v>
       </c>
       <c r="B54" t="n">
-        <v>266.9164428710938</v>
+        <v>266.9164123535156</v>
       </c>
       <c r="C54" t="n">
-        <v>269.6540354783527</v>
+        <v>269.6540046477752</v>
       </c>
       <c r="D54" t="n">
-        <v>259.3391445844601</v>
+        <v>259.3391149332235</v>
       </c>
       <c r="E54" t="n">
-        <v>268.8718746869992</v>
+        <v>268.8718439458491</v>
       </c>
       <c r="F54" t="n">
         <v>1007637</v>
@@ -1521,16 +1521,16 @@
         <v>45006</v>
       </c>
       <c r="B55" t="n">
-        <v>261.6856384277344</v>
+        <v>261.6856689453125</v>
       </c>
       <c r="C55" t="n">
-        <v>268.5785529974847</v>
+        <v>268.5785843189093</v>
       </c>
       <c r="D55" t="n">
-        <v>260.6590487314513</v>
+        <v>260.6590791293094</v>
       </c>
       <c r="E55" t="n">
-        <v>267.8941399749497</v>
+        <v>267.8941712165585</v>
       </c>
       <c r="F55" t="n">
         <v>1330396</v>
@@ -1541,16 +1541,16 @@
         <v>45007</v>
       </c>
       <c r="B56" t="n">
-        <v>265.9386901855469</v>
+        <v>265.938720703125</v>
       </c>
       <c r="C56" t="n">
-        <v>268.4318534710294</v>
+        <v>268.4318842747085</v>
       </c>
       <c r="D56" t="n">
-        <v>263.4944007536944</v>
+        <v>263.4944309907801</v>
       </c>
       <c r="E56" t="n">
-        <v>263.7877035505097</v>
+        <v>263.7877338212531</v>
       </c>
       <c r="F56" t="n">
         <v>1083636</v>
@@ -1561,16 +1561,16 @@
         <v>45008</v>
       </c>
       <c r="B57" t="n">
-        <v>262.0278625488281</v>
+        <v>262.02783203125</v>
       </c>
       <c r="C57" t="n">
-        <v>266.525361679484</v>
+        <v>266.525330638096</v>
       </c>
       <c r="D57" t="n">
-        <v>261.3434494802965</v>
+        <v>261.3434190424298</v>
       </c>
       <c r="E57" t="n">
-        <v>263.3477849881269</v>
+        <v>263.3477543168215</v>
       </c>
       <c r="F57" t="n">
         <v>1320289</v>
@@ -1661,16 +1661,16 @@
         <v>45016</v>
       </c>
       <c r="B62" t="n">
-        <v>255.3305053710938</v>
+        <v>255.3304901123047</v>
       </c>
       <c r="C62" t="n">
-        <v>256.6993016853203</v>
+        <v>256.6992863447307</v>
       </c>
       <c r="D62" t="n">
-        <v>251.6640706878859</v>
+        <v>251.6640556482063</v>
       </c>
       <c r="E62" t="n">
-        <v>251.8107221077098</v>
+        <v>251.8107070592663</v>
       </c>
       <c r="F62" t="n">
         <v>1436959</v>
@@ -1681,16 +1681,16 @@
         <v>45019</v>
       </c>
       <c r="B63" t="n">
-        <v>260.7568054199219</v>
+        <v>260.7568359375</v>
       </c>
       <c r="C63" t="n">
-        <v>261.9789501212948</v>
+        <v>261.9789807819061</v>
       </c>
       <c r="D63" t="n">
-        <v>254.7927333097189</v>
+        <v>254.792763129294</v>
       </c>
       <c r="E63" t="n">
-        <v>258.6058188104988</v>
+        <v>258.605849076337</v>
       </c>
       <c r="F63" t="n">
         <v>1008929</v>
@@ -1701,16 +1701,16 @@
         <v>45021</v>
       </c>
       <c r="B64" t="n">
-        <v>261.4901428222656</v>
+        <v>261.4901123046875</v>
       </c>
       <c r="C64" t="n">
-        <v>262.7122877600449</v>
+        <v>262.7122570998346</v>
       </c>
       <c r="D64" t="n">
-        <v>257.4325977588201</v>
+        <v>257.4325677147835</v>
       </c>
       <c r="E64" t="n">
-        <v>261.4412391222407</v>
+        <v>261.44120861037</v>
       </c>
       <c r="F64" t="n">
         <v>1884700</v>
@@ -1741,16 +1741,16 @@
         <v>45026</v>
       </c>
       <c r="B66" t="n">
-        <v>260.8056945800781</v>
+        <v>260.8057250976562</v>
       </c>
       <c r="C66" t="n">
-        <v>262.4189197130697</v>
+        <v>262.4189504194156</v>
       </c>
       <c r="D66" t="n">
-        <v>259.6813273563276</v>
+        <v>259.6813577423405</v>
       </c>
       <c r="E66" t="n">
-        <v>260.0724077162166</v>
+        <v>260.0724381479909</v>
       </c>
       <c r="F66" t="n">
         <v>722146</v>
@@ -1761,16 +1761,16 @@
         <v>45027</v>
       </c>
       <c r="B67" t="n">
-        <v>259.8768310546875</v>
+        <v>259.8768920898438</v>
       </c>
       <c r="C67" t="n">
-        <v>263.2499622835784</v>
+        <v>263.2500241109545</v>
       </c>
       <c r="D67" t="n">
-        <v>259.0946703998079</v>
+        <v>259.0947312512644</v>
       </c>
       <c r="E67" t="n">
-        <v>261.5389597432023</v>
+        <v>261.5390211687292</v>
       </c>
       <c r="F67" t="n">
         <v>852555</v>
@@ -1801,16 +1801,16 @@
         <v>45029</v>
       </c>
       <c r="B69" t="n">
-        <v>257.2370300292969</v>
+        <v>257.237060546875</v>
       </c>
       <c r="C69" t="n">
-        <v>263.1033247627471</v>
+        <v>263.1033559762791</v>
       </c>
       <c r="D69" t="n">
-        <v>256.3081880948267</v>
+        <v>256.3082185022108</v>
       </c>
       <c r="E69" t="n">
-        <v>261.3434184402013</v>
+        <v>261.343449444945</v>
       </c>
       <c r="F69" t="n">
         <v>1119774</v>
@@ -1821,16 +1821,16 @@
         <v>45033</v>
       </c>
       <c r="B70" t="n">
-        <v>252.7884063720703</v>
+        <v>252.7884216308594</v>
       </c>
       <c r="C70" t="n">
-        <v>254.0105511134505</v>
+        <v>254.0105664460105</v>
       </c>
       <c r="D70" t="n">
-        <v>246.2866023154313</v>
+        <v>246.2866171817591</v>
       </c>
       <c r="E70" t="n">
-        <v>251.7618167243182</v>
+        <v>251.7618319211404</v>
       </c>
       <c r="F70" t="n">
         <v>1947730</v>
@@ -1881,16 +1881,16 @@
         <v>45036</v>
       </c>
       <c r="B73" t="n">
-        <v>253.1305999755859</v>
+        <v>253.130615234375</v>
       </c>
       <c r="C73" t="n">
-        <v>254.4505221965584</v>
+        <v>254.4505375349128</v>
       </c>
       <c r="D73" t="n">
-        <v>250.9796432428128</v>
+        <v>250.9796583719415</v>
       </c>
       <c r="E73" t="n">
-        <v>252.4950907099374</v>
+        <v>252.4951059304178</v>
       </c>
       <c r="F73" t="n">
         <v>903815</v>
@@ -1901,16 +1901,16 @@
         <v>45037</v>
       </c>
       <c r="B74" t="n">
-        <v>251.2729644775391</v>
+        <v>251.2729797363281</v>
       </c>
       <c r="C74" t="n">
-        <v>254.6460959745991</v>
+        <v>254.6461114382248</v>
       </c>
       <c r="D74" t="n">
-        <v>250.0997084831857</v>
+        <v>250.0997236707277</v>
       </c>
       <c r="E74" t="n">
-        <v>253.6194764662458</v>
+        <v>253.619491867529</v>
       </c>
       <c r="F74" t="n">
         <v>911187</v>
@@ -1941,16 +1941,16 @@
         <v>45041</v>
       </c>
       <c r="B76" t="n">
-        <v>259.3391418457031</v>
+        <v>259.3390808105469</v>
       </c>
       <c r="C76" t="n">
-        <v>263.738863385027</v>
+        <v>263.7388013144016</v>
       </c>
       <c r="D76" t="n">
-        <v>255.428278255193</v>
+        <v>255.4282181404538</v>
       </c>
       <c r="E76" t="n">
-        <v>259.2902679858303</v>
+        <v>259.2902069621764</v>
       </c>
       <c r="F76" t="n">
         <v>1594968</v>
@@ -1961,16 +1961,16 @@
         <v>45042</v>
       </c>
       <c r="B77" t="n">
-        <v>261.4901428222656</v>
+        <v>261.4901123046875</v>
       </c>
       <c r="C77" t="n">
-        <v>262.5167326349911</v>
+        <v>262.5167019976033</v>
       </c>
       <c r="D77" t="n">
-        <v>258.1170108589856</v>
+        <v>258.1169807350737</v>
       </c>
       <c r="E77" t="n">
-        <v>259.0947268092091</v>
+        <v>259.0946965711914</v>
       </c>
       <c r="F77" t="n">
         <v>845386</v>
@@ -1981,16 +1981,16 @@
         <v>45043</v>
       </c>
       <c r="B78" t="n">
-        <v>265.1565551757812</v>
+        <v>265.1565246582031</v>
       </c>
       <c r="C78" t="n">
-        <v>269.1651663621336</v>
+        <v>269.1651353831937</v>
       </c>
       <c r="D78" t="n">
-        <v>258.8502758959981</v>
+        <v>258.8502461042265</v>
       </c>
       <c r="E78" t="n">
-        <v>262.0278524650707</v>
+        <v>262.0278223075834</v>
       </c>
       <c r="F78" t="n">
         <v>2306301</v>
@@ -2001,16 +2001,16 @@
         <v>45044</v>
       </c>
       <c r="B79" t="n">
-        <v>266.8675537109375</v>
+        <v>266.8675231933594</v>
       </c>
       <c r="C79" t="n">
-        <v>271.7561329704343</v>
+        <v>271.7561018938238</v>
       </c>
       <c r="D79" t="n">
-        <v>265.3032023803946</v>
+        <v>265.3031720417075</v>
       </c>
       <c r="E79" t="n">
-        <v>266.9164275685245</v>
+        <v>266.9163970453574</v>
       </c>
       <c r="F79" t="n">
         <v>2199682</v>
@@ -2021,16 +2021,16 @@
         <v>45048</v>
       </c>
       <c r="B80" t="n">
-        <v>272.0983276367188</v>
+        <v>272.0982971191406</v>
       </c>
       <c r="C80" t="n">
-        <v>274.1515370289469</v>
+        <v>274.1515062810881</v>
       </c>
       <c r="D80" t="n">
-        <v>266.9653190749093</v>
+        <v>266.9652891330311</v>
       </c>
       <c r="E80" t="n">
-        <v>268.383019088894</v>
+        <v>268.3829889880116</v>
       </c>
       <c r="F80" t="n">
         <v>2686833</v>
@@ -2041,16 +2041,16 @@
         <v>45049</v>
       </c>
       <c r="B81" t="n">
-        <v>269.4096069335938</v>
+        <v>269.4095764160156</v>
       </c>
       <c r="C81" t="n">
-        <v>273.2227228507442</v>
+        <v>273.2226919012325</v>
       </c>
       <c r="D81" t="n">
-        <v>267.454175114551</v>
+        <v>267.454144818476</v>
       </c>
       <c r="E81" t="n">
-        <v>272.2450069412229</v>
+        <v>272.2449761024627</v>
       </c>
       <c r="F81" t="n">
         <v>1040500</v>
@@ -2201,16 +2201,16 @@
         <v>45061</v>
       </c>
       <c r="B89" t="n">
-        <v>301.7231140136719</v>
+        <v>301.7230834960938</v>
       </c>
       <c r="C89" t="n">
-        <v>302.8474812615053</v>
+        <v>302.8474506302038</v>
       </c>
       <c r="D89" t="n">
-        <v>297.2256151848188</v>
+        <v>297.2255851221371</v>
       </c>
       <c r="E89" t="n">
-        <v>301.8208915651181</v>
+        <v>301.8208610376504</v>
       </c>
       <c r="F89" t="n">
         <v>2054933</v>
@@ -2221,16 +2221,16 @@
         <v>45062</v>
       </c>
       <c r="B90" t="n">
-        <v>321.032958984375</v>
+        <v>321.0330200195312</v>
       </c>
       <c r="C90" t="n">
-        <v>327.0459046265986</v>
+        <v>327.045966804943</v>
       </c>
       <c r="D90" t="n">
-        <v>300.9897869519527</v>
+        <v>300.989844176478</v>
       </c>
       <c r="E90" t="n">
-        <v>302.6030119041324</v>
+        <v>302.6030694353658</v>
       </c>
       <c r="F90" t="n">
         <v>16881729</v>
@@ -2241,16 +2241,16 @@
         <v>45063</v>
       </c>
       <c r="B91" t="n">
-        <v>313.8956604003906</v>
+        <v>313.8956909179688</v>
       </c>
       <c r="C91" t="n">
-        <v>320.6907974646027</v>
+        <v>320.690828642818</v>
       </c>
       <c r="D91" t="n">
-        <v>309.3981913791345</v>
+        <v>309.3982214594595</v>
       </c>
       <c r="E91" t="n">
-        <v>320.6907974646027</v>
+        <v>320.690828642818</v>
       </c>
       <c r="F91" t="n">
         <v>5372474</v>
@@ -2301,16 +2301,16 @@
         <v>45068</v>
       </c>
       <c r="B94" t="n">
-        <v>332.5211486816406</v>
+        <v>332.5211791992188</v>
       </c>
       <c r="C94" t="n">
-        <v>333.4010869318457</v>
+        <v>333.4011175301813</v>
       </c>
       <c r="D94" t="n">
-        <v>324.797199849257</v>
+        <v>324.7972296579592</v>
       </c>
       <c r="E94" t="n">
-        <v>327.1925856505085</v>
+        <v>327.1926156790506</v>
       </c>
       <c r="F94" t="n">
         <v>3643637</v>
@@ -2361,16 +2361,16 @@
         <v>45071</v>
       </c>
       <c r="B97" t="n">
-        <v>327.9259033203125</v>
+        <v>327.9258728027344</v>
       </c>
       <c r="C97" t="n">
-        <v>331.8367668777104</v>
+        <v>331.8367359961779</v>
       </c>
       <c r="D97" t="n">
-        <v>320.0553023460575</v>
+        <v>320.0552725609366</v>
       </c>
       <c r="E97" t="n">
-        <v>324.1128173193537</v>
+        <v>324.1127871566306</v>
       </c>
       <c r="F97" t="n">
         <v>2917161</v>
@@ -2401,16 +2401,16 @@
         <v>45075</v>
       </c>
       <c r="B99" t="n">
-        <v>331.9833984375</v>
+        <v>331.9834289550781</v>
       </c>
       <c r="C99" t="n">
-        <v>335.7476103538602</v>
+        <v>335.7476412174635</v>
       </c>
       <c r="D99" t="n">
-        <v>329.0013770883488</v>
+        <v>329.0014073318046</v>
       </c>
       <c r="E99" t="n">
-        <v>335.2098785818884</v>
+        <v>335.2099093960608</v>
       </c>
       <c r="F99" t="n">
         <v>3389349</v>
@@ -2441,16 +2441,16 @@
         <v>45077</v>
       </c>
       <c r="B101" t="n">
-        <v>335.8453979492188</v>
+        <v>335.8453674316406</v>
       </c>
       <c r="C101" t="n">
-        <v>337.31197173939</v>
+        <v>337.3119410885474</v>
       </c>
       <c r="D101" t="n">
-        <v>326.5570972781341</v>
+        <v>326.5570676045647</v>
       </c>
       <c r="E101" t="n">
-        <v>329.1969420354504</v>
+        <v>329.1969121220038</v>
       </c>
       <c r="F101" t="n">
         <v>3074082</v>
@@ -2501,16 +2501,16 @@
         <v>45082</v>
       </c>
       <c r="B104" t="n">
-        <v>338.7296752929688</v>
+        <v>338.7296447753906</v>
       </c>
       <c r="C104" t="n">
-        <v>346.1114181807419</v>
+        <v>346.1113869981116</v>
       </c>
       <c r="D104" t="n">
-        <v>337.0675463779966</v>
+        <v>337.0675160101666</v>
       </c>
       <c r="E104" t="n">
-        <v>343.4715733952027</v>
+        <v>343.471542450407</v>
       </c>
       <c r="F104" t="n">
         <v>1932526</v>
@@ -2521,16 +2521,16 @@
         <v>45083</v>
       </c>
       <c r="B105" t="n">
-        <v>335.894287109375</v>
+        <v>335.8942565917969</v>
       </c>
       <c r="C105" t="n">
-        <v>338.2897030107895</v>
+        <v>338.2896722755765</v>
       </c>
       <c r="D105" t="n">
-        <v>324.7972354615527</v>
+        <v>324.797205952194</v>
       </c>
       <c r="E105" t="n">
-        <v>338.2897030107895</v>
+        <v>338.2896722755765</v>
       </c>
       <c r="F105" t="n">
         <v>4504948</v>
@@ -2581,16 +2581,16 @@
         <v>45086</v>
       </c>
       <c r="B108" t="n">
-        <v>321.1796569824219</v>
+        <v>321.1796875</v>
       </c>
       <c r="C108" t="n">
-        <v>329.7835445343098</v>
+        <v>329.7835758694049</v>
       </c>
       <c r="D108" t="n">
-        <v>319.8108607588288</v>
+        <v>319.8108911463478</v>
       </c>
       <c r="E108" t="n">
-        <v>328.4636520057679</v>
+        <v>328.4636832154505</v>
       </c>
       <c r="F108" t="n">
         <v>1069100</v>
@@ -2661,16 +2661,16 @@
         <v>45092</v>
       </c>
       <c r="B112" t="n">
-        <v>327.4859313964844</v>
+        <v>327.4859619140625</v>
       </c>
       <c r="C112" t="n">
-        <v>332.6189395385138</v>
+        <v>332.6189705344239</v>
       </c>
       <c r="D112" t="n">
-        <v>326.7526445190516</v>
+        <v>326.7526749682966</v>
       </c>
       <c r="E112" t="n">
-        <v>329.9302209879269</v>
+        <v>329.9302517332822</v>
       </c>
       <c r="F112" t="n">
         <v>1135497</v>
@@ -2681,16 +2681,16 @@
         <v>45093</v>
       </c>
       <c r="B113" t="n">
-        <v>332.1300964355469</v>
+        <v>332.1300659179688</v>
       </c>
       <c r="C113" t="n">
-        <v>338.1919169902123</v>
+        <v>338.1918859156474</v>
       </c>
       <c r="D113" t="n">
-        <v>329.0013936839306</v>
+        <v>329.0013634538315</v>
       </c>
       <c r="E113" t="n">
-        <v>329.0013936839306</v>
+        <v>329.0013634538315</v>
       </c>
       <c r="F113" t="n">
         <v>3232641</v>
@@ -2741,16 +2741,16 @@
         <v>45098</v>
       </c>
       <c r="B116" t="n">
-        <v>331.9833984375</v>
+        <v>331.9834289550781</v>
       </c>
       <c r="C116" t="n">
-        <v>334.6721169723974</v>
+        <v>334.672147737136</v>
       </c>
       <c r="D116" t="n">
-        <v>330.4679508346564</v>
+        <v>330.467981212927</v>
       </c>
       <c r="E116" t="n">
-        <v>330.5168246911924</v>
+        <v>330.5168550739557</v>
       </c>
       <c r="F116" t="n">
         <v>981946</v>
@@ -2761,16 +2761,16 @@
         <v>45099</v>
       </c>
       <c r="B117" t="n">
-        <v>336.52978515625</v>
+        <v>336.5298156738281</v>
       </c>
       <c r="C117" t="n">
-        <v>338.2896616343696</v>
+        <v>338.2896923115389</v>
       </c>
       <c r="D117" t="n">
-        <v>327.6325655446055</v>
+        <v>327.6325952553558</v>
       </c>
       <c r="E117" t="n">
-        <v>331.9833828856582</v>
+        <v>331.9834129909543</v>
       </c>
       <c r="F117" t="n">
         <v>2659471</v>
@@ -2781,16 +2781,16 @@
         <v>45100</v>
       </c>
       <c r="B118" t="n">
-        <v>336.0409851074219</v>
+        <v>336.0409240722656</v>
       </c>
       <c r="C118" t="n">
-        <v>342.200583678628</v>
+        <v>342.2005215247033</v>
       </c>
       <c r="D118" t="n">
-        <v>332.2278690192702</v>
+        <v>332.2278086766906</v>
       </c>
       <c r="E118" t="n">
-        <v>341.2228677252605</v>
+        <v>341.2228057489184</v>
       </c>
       <c r="F118" t="n">
         <v>5871422</v>
@@ -2801,16 +2801,16 @@
         <v>45103</v>
       </c>
       <c r="B119" t="n">
-        <v>332.5700073242188</v>
+        <v>332.570068359375</v>
       </c>
       <c r="C119" t="n">
-        <v>335.0142967060482</v>
+        <v>335.0143581897945</v>
       </c>
       <c r="D119" t="n">
-        <v>327.5836510177832</v>
+        <v>327.5837111378147</v>
       </c>
       <c r="E119" t="n">
-        <v>335.0142967060482</v>
+        <v>335.0143581897945</v>
       </c>
       <c r="F119" t="n">
         <v>1283233</v>
@@ -2841,16 +2841,16 @@
         <v>45105</v>
       </c>
       <c r="B121" t="n">
-        <v>343.9115905761719</v>
+        <v>343.9115295410156</v>
       </c>
       <c r="C121" t="n">
-        <v>348.0668834260617</v>
+        <v>348.0668216534515</v>
       </c>
       <c r="D121" t="n">
-        <v>339.8540752902547</v>
+        <v>339.8540149751995</v>
       </c>
       <c r="E121" t="n">
-        <v>346.2092290606744</v>
+        <v>346.2091676177485</v>
       </c>
       <c r="F121" t="n">
         <v>2091878</v>
@@ -2861,16 +2861,16 @@
         <v>45107</v>
       </c>
       <c r="B122" t="n">
-        <v>350.9021911621094</v>
+        <v>350.9022216796875</v>
       </c>
       <c r="C122" t="n">
-        <v>355.2530383638393</v>
+        <v>355.2530692598058</v>
       </c>
       <c r="D122" t="n">
-        <v>344.7914674728921</v>
+        <v>344.7914974590273</v>
       </c>
       <c r="E122" t="n">
-        <v>345.1825478214984</v>
+        <v>345.1825778416454</v>
       </c>
       <c r="F122" t="n">
         <v>4356450</v>
@@ -2881,16 +2881,16 @@
         <v>45110</v>
       </c>
       <c r="B123" t="n">
-        <v>346.3558654785156</v>
+        <v>346.3558349609375</v>
       </c>
       <c r="C123" t="n">
-        <v>355.9374695821503</v>
+        <v>355.9374382203325</v>
       </c>
       <c r="D123" t="n">
-        <v>345.6225785367827</v>
+        <v>345.6225480838148</v>
       </c>
       <c r="E123" t="n">
-        <v>352.9065740930052</v>
+        <v>352.906542998241</v>
       </c>
       <c r="F123" t="n">
         <v>1734803</v>
@@ -2901,16 +2901,16 @@
         <v>45111</v>
       </c>
       <c r="B124" t="n">
-        <v>346.0625</v>
+        <v>346.0625305175781</v>
       </c>
       <c r="C124" t="n">
-        <v>349.3378238768937</v>
+        <v>349.3378546833068</v>
       </c>
       <c r="D124" t="n">
-        <v>342.4938136594761</v>
+        <v>342.493843862349</v>
       </c>
       <c r="E124" t="n">
-        <v>346.355802788597</v>
+        <v>346.35583333204</v>
       </c>
       <c r="F124" t="n">
         <v>1341376</v>
@@ -2961,16 +2961,16 @@
         <v>45114</v>
       </c>
       <c r="B127" t="n">
-        <v>346.7958374023438</v>
+        <v>346.7958068847656</v>
       </c>
       <c r="C127" t="n">
-        <v>352.5154514770236</v>
+        <v>352.5154204561269</v>
       </c>
       <c r="D127" t="n">
-        <v>345.1825823171561</v>
+        <v>345.1825519415423</v>
       </c>
       <c r="E127" t="n">
-        <v>348.0668561217124</v>
+        <v>348.0668254922863</v>
       </c>
       <c r="F127" t="n">
         <v>2437598</v>
@@ -2981,16 +2981,16 @@
         <v>45117</v>
       </c>
       <c r="B128" t="n">
-        <v>338.2407836914062</v>
+        <v>338.2408447265625</v>
       </c>
       <c r="C128" t="n">
-        <v>347.7246087894365</v>
+        <v>347.724671535938</v>
       </c>
       <c r="D128" t="n">
-        <v>335.9431456567614</v>
+        <v>335.9432062773116</v>
       </c>
       <c r="E128" t="n">
-        <v>347.5290835372967</v>
+        <v>347.5291462485159</v>
       </c>
       <c r="F128" t="n">
         <v>1895779</v>
@@ -3001,16 +3001,16 @@
         <v>45118</v>
       </c>
       <c r="B129" t="n">
-        <v>347.2357482910156</v>
+        <v>347.2358093261719</v>
       </c>
       <c r="C129" t="n">
-        <v>348.1645902036252</v>
+        <v>348.1646514020481</v>
       </c>
       <c r="D129" t="n">
-        <v>337.4097167787521</v>
+        <v>337.4097760867435</v>
       </c>
       <c r="E129" t="n">
-        <v>339.267370766454</v>
+        <v>339.2674304009734</v>
       </c>
       <c r="F129" t="n">
         <v>1520560</v>
@@ -3041,16 +3041,16 @@
         <v>45120</v>
       </c>
       <c r="B131" t="n">
-        <v>353.8353271484375</v>
+        <v>353.8353576660156</v>
       </c>
       <c r="C131" t="n">
-        <v>358.283951753566</v>
+        <v>358.2839826548289</v>
       </c>
       <c r="D131" t="n">
-        <v>340.3917354647012</v>
+        <v>340.3917648227968</v>
       </c>
       <c r="E131" t="n">
-        <v>341.9072127933781</v>
+        <v>341.9072422821805</v>
       </c>
       <c r="F131" t="n">
         <v>7094935</v>
@@ -3081,16 +3081,16 @@
         <v>45124</v>
       </c>
       <c r="B133" t="n">
-        <v>377.4801330566406</v>
+        <v>377.4801025390625</v>
       </c>
       <c r="C133" t="n">
-        <v>387.0166619337575</v>
+        <v>387.0166306451937</v>
       </c>
       <c r="D133" t="n">
-        <v>370.8438762077714</v>
+        <v>370.843846226705</v>
       </c>
       <c r="E133" t="n">
-        <v>376.7919166413512</v>
+        <v>376.7918861794124</v>
       </c>
       <c r="F133" t="n">
         <v>7245327</v>
@@ -3121,16 +3121,16 @@
         <v>45126</v>
       </c>
       <c r="B135" t="n">
-        <v>386.869140625</v>
+        <v>386.8691711425781</v>
       </c>
       <c r="C135" t="n">
-        <v>391.1949903263676</v>
+        <v>391.1950211851837</v>
       </c>
       <c r="D135" t="n">
-        <v>383.4281190438373</v>
+        <v>383.4281492899758</v>
       </c>
       <c r="E135" t="n">
-        <v>386.8199951751714</v>
+        <v>386.8200256888728</v>
       </c>
       <c r="F135" t="n">
         <v>3453054</v>
@@ -3181,16 +3181,16 @@
         <v>45131</v>
       </c>
       <c r="B138" t="n">
-        <v>376.8902282714844</v>
+        <v>376.8901977539062</v>
       </c>
       <c r="C138" t="n">
-        <v>380.0854629718369</v>
+        <v>380.0854321955341</v>
       </c>
       <c r="D138" t="n">
-        <v>373.4492062864893</v>
+        <v>373.4491760475378</v>
       </c>
       <c r="E138" t="n">
-        <v>379.0039929187438</v>
+        <v>379.0039622300098</v>
       </c>
       <c r="F138" t="n">
         <v>2470379</v>
@@ -3221,16 +3221,16 @@
         <v>45133</v>
       </c>
       <c r="B140" t="n">
-        <v>372.9084167480469</v>
+        <v>372.908447265625</v>
       </c>
       <c r="C140" t="n">
-        <v>377.4800837606867</v>
+        <v>377.4801146523948</v>
       </c>
       <c r="D140" t="n">
-        <v>371.6303350046529</v>
+        <v>371.6303654176371</v>
       </c>
       <c r="E140" t="n">
-        <v>372.9575922017636</v>
+        <v>372.9576227233661</v>
       </c>
       <c r="F140" t="n">
         <v>1085762</v>
@@ -3301,16 +3301,16 @@
         <v>45139</v>
       </c>
       <c r="B144" t="n">
-        <v>424.8678894042969</v>
+        <v>424.8678588867188</v>
       </c>
       <c r="C144" t="n">
-        <v>427.5715495046408</v>
+        <v>427.5715187928632</v>
       </c>
       <c r="D144" t="n">
-        <v>412.9226335070796</v>
+        <v>412.92260384751</v>
       </c>
       <c r="E144" t="n">
-        <v>420.787826526262</v>
+        <v>420.7877963017483</v>
       </c>
       <c r="F144" t="n">
         <v>3174123</v>
@@ -3321,16 +3321,16 @@
         <v>45140</v>
       </c>
       <c r="B145" t="n">
-        <v>418.5265502929688</v>
+        <v>418.5265808105469</v>
       </c>
       <c r="C145" t="n">
-        <v>424.5237353191513</v>
+        <v>424.5237662740245</v>
       </c>
       <c r="D145" t="n">
-        <v>411.3495444367819</v>
+        <v>411.3495744310364</v>
       </c>
       <c r="E145" t="n">
-        <v>424.2288026141456</v>
+        <v>424.2288335475131</v>
       </c>
       <c r="F145" t="n">
         <v>2299029</v>
@@ -3401,16 +3401,16 @@
         <v>45146</v>
       </c>
       <c r="B149" t="n">
-        <v>443.9409484863281</v>
+        <v>443.9409790039062</v>
       </c>
       <c r="C149" t="n">
-        <v>447.0870374969841</v>
+        <v>447.087068230832</v>
       </c>
       <c r="D149" t="n">
-        <v>439.5167776919654</v>
+        <v>439.5168079054153</v>
       </c>
       <c r="E149" t="n">
-        <v>442.3679339843285</v>
+        <v>442.3679643937738</v>
       </c>
       <c r="F149" t="n">
         <v>2318513</v>
@@ -3421,16 +3421,16 @@
         <v>45147</v>
       </c>
       <c r="B150" t="n">
-        <v>446.4971313476562</v>
+        <v>446.4971618652344</v>
       </c>
       <c r="C150" t="n">
-        <v>447.8735340055565</v>
+        <v>447.8735646172102</v>
       </c>
       <c r="D150" t="n">
-        <v>439.8608753152855</v>
+        <v>439.860905379283</v>
       </c>
       <c r="E150" t="n">
-        <v>443.3510724157882</v>
+        <v>443.3511027183367</v>
       </c>
       <c r="F150" t="n">
         <v>1549021</v>
@@ -3441,16 +3441,16 @@
         <v>45148</v>
       </c>
       <c r="B151" t="n">
-        <v>437.7962646484375</v>
+        <v>437.7962951660156</v>
       </c>
       <c r="C151" t="n">
-        <v>445.0715916989516</v>
+        <v>445.0716227236729</v>
       </c>
       <c r="D151" t="n">
-        <v>437.1080783080701</v>
+        <v>437.1081087776766</v>
       </c>
       <c r="E151" t="n">
-        <v>445.0715916989516</v>
+        <v>445.0716227236729</v>
       </c>
       <c r="F151" t="n">
         <v>1661347</v>
@@ -3461,16 +3461,16 @@
         <v>45149</v>
       </c>
       <c r="B152" t="n">
-        <v>438.3370361328125</v>
+        <v>438.3370056152344</v>
       </c>
       <c r="C152" t="n">
-        <v>443.5477144078076</v>
+        <v>443.5476835274554</v>
       </c>
       <c r="D152" t="n">
-        <v>433.2738242234626</v>
+        <v>433.2737940583917</v>
       </c>
       <c r="E152" t="n">
-        <v>438.4845024984577</v>
+        <v>438.4844719706128</v>
       </c>
       <c r="F152" t="n">
         <v>1486040</v>
@@ -3481,16 +3481,16 @@
         <v>45152</v>
       </c>
       <c r="B153" t="n">
-        <v>440.5982360839844</v>
+        <v>440.5982666015625</v>
       </c>
       <c r="C153" t="n">
-        <v>441.3355978636641</v>
+        <v>441.3356284323149</v>
       </c>
       <c r="D153" t="n">
-        <v>431.2583202080407</v>
+        <v>431.2583500786993</v>
       </c>
       <c r="E153" t="n">
-        <v>437.3538562547245</v>
+        <v>437.353886547584</v>
       </c>
       <c r="F153" t="n">
         <v>1172380</v>
@@ -3501,16 +3501,16 @@
         <v>45154</v>
       </c>
       <c r="B154" t="n">
-        <v>443.9409484863281</v>
+        <v>443.9409790039062</v>
       </c>
       <c r="C154" t="n">
-        <v>446.8412502306306</v>
+        <v>446.8412809475824</v>
       </c>
       <c r="D154" t="n">
-        <v>438.7302704409657</v>
+        <v>438.7303006003492</v>
       </c>
       <c r="E154" t="n">
-        <v>442.4170794362679</v>
+        <v>442.4171098490916</v>
       </c>
       <c r="F154" t="n">
         <v>2240944</v>
@@ -3521,16 +3521,16 @@
         <v>45155</v>
       </c>
       <c r="B155" t="n">
-        <v>462.1784057617188</v>
+        <v>462.1783752441406</v>
       </c>
       <c r="C155" t="n">
-        <v>464.0463830827843</v>
+        <v>464.0463524418639</v>
       </c>
       <c r="D155" t="n">
-        <v>444.383400748768</v>
+        <v>444.3833714061917</v>
       </c>
       <c r="E155" t="n">
-        <v>445.1699080407967</v>
+        <v>445.1698786462874</v>
       </c>
       <c r="F155" t="n">
         <v>5942124</v>
@@ -3541,16 +3541,16 @@
         <v>45156</v>
       </c>
       <c r="B156" t="n">
-        <v>445.9072265625</v>
+        <v>445.9072570800781</v>
       </c>
       <c r="C156" t="n">
-        <v>462.2275063150331</v>
+        <v>462.2275379495597</v>
       </c>
       <c r="D156" t="n">
-        <v>440.6965487514875</v>
+        <v>440.6965789124505</v>
       </c>
       <c r="E156" t="n">
-        <v>462.1783608653041</v>
+        <v>462.1783924964672</v>
       </c>
       <c r="F156" t="n">
         <v>2847473</v>
@@ -3581,16 +3581,16 @@
         <v>45160</v>
       </c>
       <c r="B158" t="n">
-        <v>458.4424133300781</v>
+        <v>458.4423828125</v>
       </c>
       <c r="C158" t="n">
-        <v>461.0477824477497</v>
+        <v>461.0477517567375</v>
       </c>
       <c r="D158" t="n">
-        <v>454.6081378407322</v>
+        <v>454.608107578394</v>
       </c>
       <c r="E158" t="n">
-        <v>456.3778242227353</v>
+        <v>456.3777938425927</v>
       </c>
       <c r="F158" t="n">
         <v>1984953</v>
@@ -3601,16 +3601,16 @@
         <v>45161</v>
       </c>
       <c r="B159" t="n">
-        <v>457.8033752441406</v>
+        <v>457.8033447265625</v>
       </c>
       <c r="C159" t="n">
-        <v>463.8497362458489</v>
+        <v>463.849705325215</v>
       </c>
       <c r="D159" t="n">
-        <v>456.3286515850249</v>
+        <v>456.3286211657532</v>
       </c>
       <c r="E159" t="n">
-        <v>460.5070352858527</v>
+        <v>460.5070045880462</v>
       </c>
       <c r="F159" t="n">
         <v>966232</v>
@@ -3621,16 +3621,16 @@
         <v>45162</v>
       </c>
       <c r="B160" t="n">
-        <v>466.8974914550781</v>
+        <v>466.8975219726562</v>
       </c>
       <c r="C160" t="n">
-        <v>471.0758750393841</v>
+        <v>471.0759058300717</v>
       </c>
       <c r="D160" t="n">
-        <v>458.8356870120615</v>
+        <v>458.8357170027001</v>
       </c>
       <c r="E160" t="n">
-        <v>461.5884924309786</v>
+        <v>461.5885226015474</v>
       </c>
       <c r="F160" t="n">
         <v>2438414</v>
@@ -3641,16 +3641,16 @@
         <v>45163</v>
       </c>
       <c r="B161" t="n">
-        <v>476.3848571777344</v>
+        <v>476.3848876953125</v>
       </c>
       <c r="C161" t="n">
-        <v>479.4326252142169</v>
+        <v>479.4326559270373</v>
       </c>
       <c r="D161" t="n">
-        <v>468.8146275423792</v>
+        <v>468.8146575750027</v>
       </c>
       <c r="E161" t="n">
-        <v>469.9452429420974</v>
+        <v>469.9452730471489</v>
       </c>
       <c r="F161" t="n">
         <v>3630212</v>
@@ -3661,16 +3661,16 @@
         <v>45166</v>
       </c>
       <c r="B162" t="n">
-        <v>476.87646484375</v>
+        <v>476.8764343261719</v>
       </c>
       <c r="C162" t="n">
-        <v>480.2191958277009</v>
+        <v>480.2191650962056</v>
       </c>
       <c r="D162" t="n">
-        <v>470.2893837943881</v>
+        <v>470.2893536983485</v>
       </c>
       <c r="E162" t="n">
-        <v>477.2205730336661</v>
+        <v>477.2205424940669</v>
       </c>
       <c r="F162" t="n">
         <v>1287199</v>
@@ -3741,16 +3741,16 @@
         <v>45170</v>
       </c>
       <c r="B166" t="n">
-        <v>519.44677734375</v>
+        <v>519.4468383789062</v>
       </c>
       <c r="C166" t="n">
-        <v>521.9538554303341</v>
+        <v>521.9539167600727</v>
       </c>
       <c r="D166" t="n">
-        <v>499.4397181489117</v>
+        <v>499.4397768332323</v>
       </c>
       <c r="E166" t="n">
-        <v>504.2571725037978</v>
+        <v>504.2572317541708</v>
       </c>
       <c r="F166" t="n">
         <v>3248231</v>
@@ -3801,16 +3801,16 @@
         <v>45175</v>
       </c>
       <c r="B169" t="n">
-        <v>509.95947265625</v>
+        <v>509.9594116210938</v>
       </c>
       <c r="C169" t="n">
-        <v>521.8555532881034</v>
+        <v>521.8554908291494</v>
       </c>
       <c r="D169" t="n">
-        <v>507.1083161378745</v>
+        <v>507.1082554439625</v>
       </c>
       <c r="E169" t="n">
-        <v>515.6125802305045</v>
+        <v>515.6125185187487</v>
       </c>
       <c r="F169" t="n">
         <v>2392443</v>
@@ -3881,16 +3881,16 @@
         <v>45181</v>
       </c>
       <c r="B173" t="n">
-        <v>488.7725830078125</v>
+        <v>488.7725524902344</v>
       </c>
       <c r="C173" t="n">
-        <v>510.8934683921963</v>
+        <v>510.8934364934527</v>
       </c>
       <c r="D173" t="n">
-        <v>486.1180983640842</v>
+        <v>486.1180680122447</v>
       </c>
       <c r="E173" t="n">
-        <v>503.8147826689271</v>
+        <v>503.8147512121566</v>
       </c>
       <c r="F173" t="n">
         <v>3948677</v>
@@ -3921,16 +3921,16 @@
         <v>45183</v>
       </c>
       <c r="B175" t="n">
-        <v>497.2276306152344</v>
+        <v>497.2276611328125</v>
       </c>
       <c r="C175" t="n">
-        <v>505.3386102545338</v>
+        <v>505.3386412699271</v>
       </c>
       <c r="D175" t="n">
-        <v>487.9368601179784</v>
+        <v>487.9368900653312</v>
       </c>
       <c r="E175" t="n">
-        <v>489.0675055249067</v>
+        <v>489.0675355416533</v>
       </c>
       <c r="F175" t="n">
         <v>3601415</v>
@@ -3981,16 +3981,16 @@
         <v>45189</v>
       </c>
       <c r="B178" t="n">
-        <v>476.8273315429688</v>
+        <v>476.8273010253906</v>
       </c>
       <c r="C178" t="n">
-        <v>486.3147147163019</v>
+        <v>486.3146835915187</v>
       </c>
       <c r="D178" t="n">
-        <v>473.1896677339891</v>
+        <v>473.1896374492263</v>
       </c>
       <c r="E178" t="n">
-        <v>479.7767789545747</v>
+        <v>479.776748248228</v>
       </c>
       <c r="F178" t="n">
         <v>1886250</v>
@@ -4041,16 +4041,16 @@
         <v>45194</v>
       </c>
       <c r="B181" t="n">
-        <v>480.1699829101562</v>
+        <v>480.1700134277344</v>
       </c>
       <c r="C181" t="n">
-        <v>488.0351751937078</v>
+        <v>488.0352062111644</v>
       </c>
       <c r="D181" t="n">
-        <v>476.8272821903123</v>
+        <v>476.8273124954425</v>
       </c>
       <c r="E181" t="n">
-        <v>481.5463855591123</v>
+        <v>481.5464161641688</v>
       </c>
       <c r="F181" t="n">
         <v>1287496</v>
@@ -4061,16 +4061,16 @@
         <v>45195</v>
       </c>
       <c r="B182" t="n">
-        <v>475.5983581542969</v>
+        <v>475.598388671875</v>
       </c>
       <c r="C182" t="n">
-        <v>484.1517669844497</v>
+        <v>484.1517980508718</v>
       </c>
       <c r="D182" t="n">
-        <v>474.8118509070009</v>
+        <v>474.8118813741115</v>
       </c>
       <c r="E182" t="n">
-        <v>481.2023198020975</v>
+        <v>481.2023506792632</v>
       </c>
       <c r="F182" t="n">
         <v>931591</v>
@@ -4081,16 +4081,16 @@
         <v>45196</v>
       </c>
       <c r="B183" t="n">
-        <v>483.2177734375</v>
+        <v>483.2177429199219</v>
       </c>
       <c r="C183" t="n">
-        <v>484.6924970593846</v>
+        <v>484.6924664486704</v>
       </c>
       <c r="D183" t="n">
-        <v>469.9452608405392</v>
+        <v>469.9452311611855</v>
       </c>
       <c r="E183" t="n">
-        <v>473.287961716145</v>
+        <v>473.2879318256833</v>
       </c>
       <c r="F183" t="n">
         <v>1605406</v>
@@ -4121,16 +4121,16 @@
         <v>45198</v>
       </c>
       <c r="B185" t="n">
-        <v>475.205078125</v>
+        <v>475.2051086425781</v>
       </c>
       <c r="C185" t="n">
-        <v>481.1531176108986</v>
+        <v>481.1531485104586</v>
       </c>
       <c r="D185" t="n">
-        <v>467.9789269291059</v>
+        <v>467.978956982622</v>
       </c>
       <c r="E185" t="n">
-        <v>469.3553295370555</v>
+        <v>469.355359678964</v>
       </c>
       <c r="F185" t="n">
         <v>1618689</v>
@@ -4161,16 +4161,16 @@
         <v>45203</v>
       </c>
       <c r="B187" t="n">
-        <v>483.1194152832031</v>
+        <v>483.1194763183594</v>
       </c>
       <c r="C187" t="n">
-        <v>489.3624174685501</v>
+        <v>489.3624792924194</v>
       </c>
       <c r="D187" t="n">
-        <v>471.9115226216053</v>
+        <v>471.9115822408063</v>
       </c>
       <c r="E187" t="n">
-        <v>487.5927612600497</v>
+        <v>487.5928228603486</v>
       </c>
       <c r="F187" t="n">
         <v>1785367</v>
@@ -4221,16 +4221,16 @@
         <v>45208</v>
       </c>
       <c r="B190" t="n">
-        <v>507.0591125488281</v>
+        <v>507.0591430664062</v>
       </c>
       <c r="C190" t="n">
-        <v>515.858308374322</v>
+        <v>515.8583394214836</v>
       </c>
       <c r="D190" t="n">
-        <v>497.5717304038878</v>
+        <v>497.5717603504636</v>
       </c>
       <c r="E190" t="n">
-        <v>498.4565585307918</v>
+        <v>498.4565885306214</v>
       </c>
       <c r="F190" t="n">
         <v>3470714</v>
@@ -4241,16 +4241,16 @@
         <v>45209</v>
       </c>
       <c r="B191" t="n">
-        <v>530.015625</v>
+        <v>530.0156860351562</v>
       </c>
       <c r="C191" t="n">
-        <v>534.5381466011223</v>
+        <v>534.5382081570798</v>
       </c>
       <c r="D191" t="n">
-        <v>506.960827950395</v>
+        <v>506.9608863306236</v>
       </c>
       <c r="E191" t="n">
-        <v>508.1405587964956</v>
+        <v>508.1406173125787</v>
       </c>
       <c r="F191" t="n">
         <v>6462169</v>
@@ -4261,16 +4261,16 @@
         <v>45210</v>
       </c>
       <c r="B192" t="n">
-        <v>531.0480346679688</v>
+        <v>531.0479736328125</v>
       </c>
       <c r="C192" t="n">
-        <v>539.2573060259544</v>
+        <v>539.2572440472787</v>
       </c>
       <c r="D192" t="n">
-        <v>527.2137289998506</v>
+        <v>527.2136684053842</v>
       </c>
       <c r="E192" t="n">
-        <v>533.8499857285201</v>
+        <v>533.8499243713261</v>
       </c>
       <c r="F192" t="n">
         <v>3418506</v>
@@ -4341,16 +4341,16 @@
         <v>45216</v>
       </c>
       <c r="B196" t="n">
-        <v>545.1561889648438</v>
+        <v>545.1561279296875</v>
       </c>
       <c r="C196" t="n">
-        <v>547.3682744926542</v>
+        <v>547.3682132098349</v>
       </c>
       <c r="D196" t="n">
-        <v>531.981966707664</v>
+        <v>531.9819071474808</v>
       </c>
       <c r="E196" t="n">
-        <v>535.3246977301307</v>
+        <v>535.3246377956985</v>
       </c>
       <c r="F196" t="n">
         <v>2739949</v>
@@ -4361,16 +4361,16 @@
         <v>45217</v>
       </c>
       <c r="B197" t="n">
-        <v>537.4384765625</v>
+        <v>537.4385375976562</v>
       </c>
       <c r="C197" t="n">
-        <v>550.5634929726671</v>
+        <v>550.5635554983892</v>
       </c>
       <c r="D197" t="n">
-        <v>534.6364656389118</v>
+        <v>534.6365263558527</v>
       </c>
       <c r="E197" t="n">
-        <v>548.5480493300811</v>
+        <v>548.5481116269157</v>
       </c>
       <c r="F197" t="n">
         <v>3051782</v>
@@ -4421,16 +4421,16 @@
         <v>45222</v>
       </c>
       <c r="B200" t="n">
-        <v>517.578857421875</v>
+        <v>517.5787963867188</v>
       </c>
       <c r="C200" t="n">
-        <v>539.011495871997</v>
+        <v>539.0114323094106</v>
       </c>
       <c r="D200" t="n">
-        <v>514.0394846460798</v>
+        <v>514.0394240283018</v>
       </c>
       <c r="E200" t="n">
-        <v>537.6842685852357</v>
+        <v>537.6842051791617</v>
       </c>
       <c r="F200" t="n">
         <v>1728468</v>
@@ -4441,16 +4441,16 @@
         <v>45224</v>
       </c>
       <c r="B201" t="n">
-        <v>516.4481811523438</v>
+        <v>516.4482421875</v>
       </c>
       <c r="C201" t="n">
-        <v>525.9355934358607</v>
+        <v>525.9356555922634</v>
       </c>
       <c r="D201" t="n">
-        <v>511.4341450273004</v>
+        <v>511.4342054698851</v>
       </c>
       <c r="E201" t="n">
-        <v>517.5788265563514</v>
+        <v>517.5788877251301</v>
       </c>
       <c r="F201" t="n">
         <v>1054661</v>
@@ -4481,16 +4481,16 @@
         <v>45226</v>
       </c>
       <c r="B203" t="n">
-        <v>533.2601318359375</v>
+        <v>533.2600708007812</v>
       </c>
       <c r="C203" t="n">
-        <v>534.2924264592822</v>
+        <v>534.2923653059729</v>
       </c>
       <c r="D203" t="n">
-        <v>520.085909004058</v>
+        <v>520.0858494767789</v>
       </c>
       <c r="E203" t="n">
-        <v>525.9356585452283</v>
+        <v>525.9355983484065</v>
       </c>
       <c r="F203" t="n">
         <v>1436568</v>
@@ -4541,16 +4541,16 @@
         <v>45231</v>
       </c>
       <c r="B206" t="n">
-        <v>564.5242309570312</v>
+        <v>564.524169921875</v>
       </c>
       <c r="C206" t="n">
-        <v>573.4708638552676</v>
+        <v>573.4708018528205</v>
       </c>
       <c r="D206" t="n">
-        <v>535.0297576573604</v>
+        <v>535.0296998110838</v>
       </c>
       <c r="E206" t="n">
-        <v>551.9890798046712</v>
+        <v>551.9890201247888</v>
       </c>
       <c r="F206" t="n">
         <v>13001342</v>
@@ -4581,16 +4581,16 @@
         <v>45233</v>
       </c>
       <c r="B208" t="n">
-        <v>577.8458251953125</v>
+        <v>577.8458862304688</v>
       </c>
       <c r="C208" t="n">
-        <v>583.0073574492902</v>
+        <v>583.007419029635</v>
       </c>
       <c r="D208" t="n">
-        <v>569.243271438683</v>
+        <v>569.2433315651917</v>
       </c>
       <c r="E208" t="n">
-        <v>570.2264204394406</v>
+        <v>570.2264806697948</v>
       </c>
       <c r="F208" t="n">
         <v>3063927</v>
@@ -4681,16 +4681,16 @@
         <v>45240</v>
       </c>
       <c r="B213" t="n">
-        <v>577.5258178710938</v>
+        <v>577.52587890625</v>
       </c>
       <c r="C213" t="n">
-        <v>587.9200942404458</v>
+        <v>587.9201563741093</v>
       </c>
       <c r="D213" t="n">
-        <v>574.1600280213499</v>
+        <v>574.1600887007966</v>
       </c>
       <c r="E213" t="n">
-        <v>578.7136868339696</v>
+        <v>578.7137479946645</v>
       </c>
       <c r="F213" t="n">
         <v>2069707</v>
@@ -4701,16 +4701,16 @@
         <v>45243</v>
       </c>
       <c r="B214" t="n">
-        <v>577.3773803710938</v>
+        <v>577.3773193359375</v>
       </c>
       <c r="C214" t="n">
-        <v>587.029209704344</v>
+        <v>587.0291476488828</v>
       </c>
       <c r="D214" t="n">
-        <v>575.7935145974697</v>
+        <v>575.7934537297454</v>
       </c>
       <c r="E214" t="n">
-        <v>586.0392784906772</v>
+        <v>586.0392165398629</v>
       </c>
       <c r="F214" t="n">
         <v>806673</v>
@@ -4841,16 +4841,16 @@
         <v>45253</v>
       </c>
       <c r="B221" t="n">
-        <v>615.9351806640625</v>
+        <v>615.9352416992188</v>
       </c>
       <c r="C221" t="n">
-        <v>625.0425594324253</v>
+        <v>625.0426213700633</v>
       </c>
       <c r="D221" t="n">
-        <v>611.9259715447939</v>
+        <v>611.9260321826637</v>
       </c>
       <c r="E221" t="n">
-        <v>620.7858071022209</v>
+        <v>620.7858686180425</v>
       </c>
       <c r="F221" t="n">
         <v>851855</v>
@@ -4881,16 +4881,16 @@
         <v>45258</v>
       </c>
       <c r="B223" t="n">
-        <v>605.5409545898438</v>
+        <v>605.5408935546875</v>
       </c>
       <c r="C223" t="n">
-        <v>612.1239611160681</v>
+        <v>612.1238994173815</v>
       </c>
       <c r="D223" t="n">
-        <v>594.0577158966314</v>
+        <v>594.0576560189216</v>
       </c>
       <c r="E223" t="n">
-        <v>611.7775093485961</v>
+        <v>611.7774476848299</v>
       </c>
       <c r="F223" t="n">
         <v>1833462</v>
@@ -5001,16 +5001,16 @@
         <v>45266</v>
       </c>
       <c r="B229" t="n">
-        <v>646.7715454101562</v>
+        <v>646.771484375</v>
       </c>
       <c r="C229" t="n">
-        <v>653.2060984097118</v>
+        <v>653.2060367673334</v>
       </c>
       <c r="D229" t="n">
-        <v>633.6054721259565</v>
+        <v>633.6054123332689</v>
       </c>
       <c r="E229" t="n">
-        <v>636.3277830103838</v>
+        <v>636.3277229607945</v>
       </c>
       <c r="F229" t="n">
         <v>3523055</v>
@@ -5081,16 +5081,16 @@
         <v>45272</v>
       </c>
       <c r="B233" t="n">
-        <v>657.2648315429688</v>
+        <v>657.2647705078125</v>
       </c>
       <c r="C233" t="n">
-        <v>663.0559048878439</v>
+        <v>663.055843314915</v>
       </c>
       <c r="D233" t="n">
-        <v>653.9980706709723</v>
+        <v>653.9980099391752</v>
       </c>
       <c r="E233" t="n">
-        <v>654.4930362703841</v>
+        <v>654.4929754926233</v>
       </c>
       <c r="F233" t="n">
         <v>1566679</v>
@@ -5121,16 +5121,16 @@
         <v>45274</v>
       </c>
       <c r="B235" t="n">
-        <v>693.3478393554688</v>
+        <v>693.3477783203125</v>
       </c>
       <c r="C235" t="n">
-        <v>699.8813611327372</v>
+        <v>699.8812995224374</v>
       </c>
       <c r="D235" t="n">
-        <v>671.3218700694667</v>
+        <v>671.3218109732485</v>
       </c>
       <c r="E235" t="n">
-        <v>673.1532186283753</v>
+        <v>673.1531593709441</v>
       </c>
       <c r="F235" t="n">
         <v>4534231</v>
@@ -5141,16 +5141,16 @@
         <v>45275</v>
       </c>
       <c r="B236" t="n">
-        <v>712.3544921875</v>
+        <v>712.3544311523438</v>
       </c>
       <c r="C236" t="n">
-        <v>723.6892169067984</v>
+        <v>723.689154900473</v>
       </c>
       <c r="D236" t="n">
-        <v>691.9619329247698</v>
+        <v>691.9618736368659</v>
       </c>
       <c r="E236" t="n">
-        <v>697.1095874283603</v>
+        <v>697.1095276994008</v>
       </c>
       <c r="F236" t="n">
         <v>5448159</v>
@@ -5161,16 +5161,16 @@
         <v>45278</v>
       </c>
       <c r="B237" t="n">
-        <v>709.2362060546875</v>
+        <v>709.2361450195312</v>
       </c>
       <c r="C237" t="n">
-        <v>720.1254490356021</v>
+        <v>720.1253870633439</v>
       </c>
       <c r="D237" t="n">
-        <v>698.6934148185603</v>
+        <v>698.6933546906913</v>
       </c>
       <c r="E237" t="n">
-        <v>711.6615495300121</v>
+        <v>711.6614882861365</v>
       </c>
       <c r="F237" t="n">
         <v>2558759</v>
@@ -5261,16 +5261,16 @@
         <v>45286</v>
       </c>
       <c r="B242" t="n">
-        <v>727.3024291992188</v>
+        <v>727.302490234375</v>
       </c>
       <c r="C242" t="n">
-        <v>738.4886391287101</v>
+        <v>738.488701102612</v>
       </c>
       <c r="D242" t="n">
-        <v>722.6002562288952</v>
+        <v>722.6003168694455</v>
       </c>
       <c r="E242" t="n">
-        <v>734.9249111510217</v>
+        <v>734.9249728258559</v>
       </c>
       <c r="F242" t="n">
         <v>1544968</v>
@@ -5281,16 +5281,16 @@
         <v>45287</v>
       </c>
       <c r="B243" t="n">
-        <v>727.5994262695312</v>
+        <v>727.599365234375</v>
       </c>
       <c r="C243" t="n">
-        <v>735.7663586052096</v>
+        <v>735.766296884965</v>
       </c>
       <c r="D243" t="n">
-        <v>719.2839800867803</v>
+        <v>719.2839197491708</v>
       </c>
       <c r="E243" t="n">
-        <v>730.5692198461416</v>
+        <v>730.5691585618623</v>
       </c>
       <c r="F243" t="n">
         <v>990093</v>

</xml_diff>